<commit_message>
correction for PolDed6All fields
</commit_message>
<xml_diff>
--- a/docs/OED_financial_terms_supported.xlsx
+++ b/docs/OED_financial_terms_supported.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\joh\Joh\07 Dev\OED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joh\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA16F4F-4325-4B39-AD4C-0AF24D71FF8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810C6BD3-C388-4D7B-B487-4BF4FF49DCCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
+    <workbookView xWindow="5220" yWindow="2430" windowWidth="21600" windowHeight="11385" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -3622,26 +3622,26 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="17" t="s">
         <v>924</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>985</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>930</v>
       </c>
@@ -3655,12 +3655,12 @@
         <v>932</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
         <v>926</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F10" s="18" t="s">
         <v>0</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" s="18" t="s">
         <v>1</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" s="18" t="s">
         <v>2</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" s="18" t="s">
         <v>911</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" s="18" t="s">
         <v>912</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
         <v>979</v>
       </c>
@@ -3733,20 +3733,20 @@
   <dimension ref="A1:E466"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <pane ySplit="1" topLeftCell="A424" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D200" sqref="D200:D203"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="68.77734375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="24" style="16" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="9" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -3850,7 +3850,7 @@
       </c>
       <c r="D8" s="16"/>
     </row>
-    <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>7</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>7</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>7</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>7</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>7</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>7</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>7</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>7</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>7</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>7</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>7</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>7</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>7</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>7</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>7</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>7</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>7</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>7</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>7</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>7</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>7</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>7</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>7</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>7</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>7</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>7</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>7</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>7</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>7</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>7</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>7</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>7</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>7</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>7</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>7</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>7</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>7</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>7</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>7</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>7</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>7</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>7</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>7</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>7</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>7</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>7</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>7</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>7</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>7</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>7</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>7</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>7</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>7</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>7</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>7</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>7</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>7</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>7</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>7</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>7</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>7</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>7</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>7</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>7</v>
       </c>
@@ -5238,7 +5238,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>7</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>7</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>7</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>7</v>
       </c>
@@ -5305,10 +5305,10 @@
         <v>229</v>
       </c>
       <c r="D113" s="16" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>7</v>
       </c>
@@ -5319,10 +5319,10 @@
         <v>231</v>
       </c>
       <c r="D114" s="16" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>7</v>
       </c>
@@ -5333,10 +5333,10 @@
         <v>233</v>
       </c>
       <c r="D115" s="16" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>7</v>
       </c>
@@ -5347,10 +5347,10 @@
         <v>235</v>
       </c>
       <c r="D116" s="16" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>7</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>7</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>7</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>7</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>7</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>7</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>7</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>7</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>7</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>7</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>7</v>
       </c>
@@ -5504,7 +5504,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>7</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>7</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>7</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>7</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>7</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>7</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>7</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>7</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>7</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>7</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>7</v>
       </c>
@@ -5658,7 +5658,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>7</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>7</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>7</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>7</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>7</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>7</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>7</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>7</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>7</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>7</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>7</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>7</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>7</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>7</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>7</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>7</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" ht="42.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>7</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="59.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>7</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>7</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>7</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>7</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>7</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>7</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>7</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>7</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>7</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>7</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>7</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>7</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>7</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>7</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>7</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>7</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>7</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>7</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>7</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>7</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>7</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>7</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
         <v>7</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
         <v>7</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
         <v>7</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
         <v>7</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
         <v>7</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
         <v>7</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
         <v>7</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
         <v>7</v>
       </c>
@@ -6301,7 +6301,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
         <v>7</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
         <v>7</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
         <v>7</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
         <v>7</v>
       </c>
@@ -6357,7 +6357,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
         <v>7</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
         <v>7</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
         <v>7</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
         <v>7</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
         <v>7</v>
       </c>
@@ -6427,7 +6427,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
         <v>7</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
         <v>7</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
         <v>7</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
         <v>7</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
         <v>7</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
         <v>7</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
         <v>7</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
         <v>7</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
         <v>7</v>
       </c>
@@ -6562,7 +6562,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
         <v>7</v>
       </c>
@@ -6576,7 +6576,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
         <v>7</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
         <v>7</v>
       </c>
@@ -6604,7 +6604,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
         <v>7</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>7</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
         <v>7</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
         <v>7</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
         <v>7</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
         <v>7</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>7</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
         <v>7</v>
       </c>
@@ -6716,7 +6716,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
         <v>7</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>7</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
         <v>7</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
         <v>7</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
         <v>7</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
         <v>7</v>
       </c>
@@ -6800,7 +6800,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
         <v>7</v>
       </c>
@@ -6817,7 +6817,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
         <v>442</v>
       </c>
@@ -6828,7 +6828,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
         <v>442</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
         <v>442</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
         <v>442</v>
       </c>
@@ -6861,7 +6861,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
         <v>442</v>
       </c>
@@ -6872,7 +6872,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="4" t="s">
         <v>442</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="4" t="s">
         <v>442</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="229" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="4" t="s">
         <v>442</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="4" t="s">
         <v>442</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="4" t="s">
         <v>442</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="232" spans="1:4" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="6" t="s">
         <v>442</v>
       </c>
@@ -6939,7 +6939,7 @@
       </c>
       <c r="D232" s="16"/>
     </row>
-    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="4" t="s">
         <v>442</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="4" t="s">
         <v>442</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="4" t="s">
         <v>442</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="4" t="s">
         <v>442</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="4" t="s">
         <v>442</v>
       </c>
@@ -6994,7 +6994,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="4" t="s">
         <v>442</v>
       </c>
@@ -7005,7 +7005,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="4" t="s">
         <v>442</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="4" t="s">
         <v>442</v>
       </c>
@@ -7027,7 +7027,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="241" spans="1:3" ht="78" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3" ht="78" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="4" t="s">
         <v>442</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="4" t="s">
         <v>442</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="78.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:3" ht="78.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="4" t="s">
         <v>442</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="4" t="s">
         <v>442</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="74.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:3" ht="74.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="4" t="s">
         <v>442</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
         <v>442</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:3" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="4" t="s">
         <v>442</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="4" t="s">
         <v>442</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:3" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="4" t="s">
         <v>442</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="4" t="s">
         <v>442</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="49.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:3" ht="49.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="4" t="s">
         <v>442</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="252" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="4" t="s">
         <v>442</v>
       </c>
@@ -7159,7 +7159,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="253" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="4" t="s">
         <v>442</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
         <v>442</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="4" t="s">
         <v>442</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="4" t="s">
         <v>442</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="257" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="4" t="s">
         <v>442</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="258" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="4" t="s">
         <v>442</v>
       </c>
@@ -7225,7 +7225,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="4" t="s">
         <v>442</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="4" t="s">
         <v>442</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="261" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="4" t="s">
         <v>442</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="4" t="s">
         <v>442</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="263" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
         <v>442</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="264" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="4" t="s">
         <v>442</v>
       </c>
@@ -7291,7 +7291,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="265" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="4" t="s">
         <v>442</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="4" t="s">
         <v>442</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="4" t="s">
         <v>442</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="4" t="s">
         <v>442</v>
       </c>
@@ -7335,7 +7335,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="6" t="s">
         <v>442</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="6" t="s">
         <v>442</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="4" t="s">
         <v>442</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="4" t="s">
         <v>442</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="273" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A273" s="4" t="s">
         <v>442</v>
       </c>
@@ -7405,7 +7405,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="4" t="s">
         <v>442</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="4" t="s">
         <v>442</v>
       </c>
@@ -7436,7 +7436,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="276" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A276" s="4" t="s">
         <v>442</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="4" t="s">
         <v>442</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="6" t="s">
         <v>442</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="6" t="s">
         <v>442</v>
       </c>
@@ -7495,7 +7495,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="6" t="s">
         <v>442</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="6" t="s">
         <v>442</v>
       </c>
@@ -7523,7 +7523,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" s="6" t="s">
         <v>442</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="283" spans="1:5" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="6" t="s">
         <v>442</v>
       </c>
@@ -7551,7 +7551,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="284" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
         <v>442</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="285" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="4" t="s">
         <v>442</v>
       </c>
@@ -7576,7 +7576,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="286" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A286" s="4" t="s">
         <v>442</v>
       </c>
@@ -7590,7 +7590,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="4" t="s">
         <v>442</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="4" t="s">
         <v>442</v>
       </c>
@@ -7618,7 +7618,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="4" t="s">
         <v>442</v>
       </c>
@@ -7632,7 +7632,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="4" t="s">
         <v>442</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="4" t="s">
         <v>442</v>
       </c>
@@ -7660,7 +7660,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="4" t="s">
         <v>442</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="4" t="s">
         <v>442</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="4" t="s">
         <v>442</v>
       </c>
@@ -7702,7 +7702,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="4" t="s">
         <v>442</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="4" t="s">
         <v>442</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="4" t="s">
         <v>442</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="4" t="s">
         <v>442</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="4" t="s">
         <v>442</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="4" t="s">
         <v>442</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="4" t="s">
         <v>442</v>
       </c>
@@ -7800,7 +7800,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="4" t="s">
         <v>442</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="4" t="s">
         <v>442</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="4" t="s">
         <v>442</v>
       </c>
@@ -7842,7 +7842,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="4" t="s">
         <v>442</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="4" t="s">
         <v>442</v>
       </c>
@@ -7870,7 +7870,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="4" t="s">
         <v>442</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" s="4" t="s">
         <v>442</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" s="4" t="s">
         <v>442</v>
       </c>
@@ -7912,7 +7912,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" s="4" t="s">
         <v>442</v>
       </c>
@@ -7926,7 +7926,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" s="4" t="s">
         <v>442</v>
       </c>
@@ -7940,7 +7940,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="4" t="s">
         <v>442</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="4" t="s">
         <v>442</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="4" t="s">
         <v>442</v>
       </c>
@@ -7982,7 +7982,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="4" t="s">
         <v>442</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="4" t="s">
         <v>442</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="4" t="s">
         <v>442</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="4" t="s">
         <v>442</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="4" t="s">
         <v>442</v>
       </c>
@@ -8052,7 +8052,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="4" t="s">
         <v>442</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="4" t="s">
         <v>442</v>
       </c>
@@ -8080,7 +8080,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="4" t="s">
         <v>442</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="4" t="s">
         <v>442</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="4" t="s">
         <v>442</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="4" t="s">
         <v>442</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="4" t="s">
         <v>442</v>
       </c>
@@ -8150,7 +8150,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="4" t="s">
         <v>442</v>
       </c>
@@ -8164,7 +8164,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="4" t="s">
         <v>442</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="4" t="s">
         <v>442</v>
       </c>
@@ -8192,7 +8192,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="4" t="s">
         <v>442</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="4" t="s">
         <v>442</v>
       </c>
@@ -8220,7 +8220,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="4" t="s">
         <v>442</v>
       </c>
@@ -8234,7 +8234,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="4" t="s">
         <v>442</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="4" t="s">
         <v>442</v>
       </c>
@@ -8262,7 +8262,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="4" t="s">
         <v>442</v>
       </c>
@@ -8276,7 +8276,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="6" t="s">
         <v>442</v>
       </c>
@@ -8293,7 +8293,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="337" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="4" t="s">
         <v>442</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="338" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="4" t="s">
         <v>442</v>
       </c>
@@ -8315,7 +8315,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="339" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="4" t="s">
         <v>442</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="340" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="4" t="s">
         <v>442</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="341" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="4" t="s">
         <v>442</v>
       </c>
@@ -8348,7 +8348,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="342" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="4" t="s">
         <v>442</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="343" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="4" t="s">
         <v>442</v>
       </c>
@@ -8370,7 +8370,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="344" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="4" t="s">
         <v>442</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="345" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="4" t="s">
         <v>442</v>
       </c>
@@ -8392,7 +8392,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="346" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="4" t="s">
         <v>442</v>
       </c>
@@ -8403,7 +8403,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="347" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="4" t="s">
         <v>442</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="348" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="4" t="s">
         <v>442</v>
       </c>
@@ -8425,7 +8425,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="349" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="6" t="s">
         <v>442</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="350" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="6" t="s">
         <v>442</v>
       </c>
@@ -8447,7 +8447,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="351" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="6" t="s">
         <v>442</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="352" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="6" t="s">
         <v>442</v>
       </c>
@@ -8469,7 +8469,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="353" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="4" t="s">
         <v>442</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="354" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="4" t="s">
         <v>442</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="355" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="4" t="s">
         <v>442</v>
       </c>
@@ -8502,7 +8502,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="356" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="4" t="s">
         <v>442</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="357" spans="1:3" ht="42.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:3" ht="42.4" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="4" t="s">
         <v>442</v>
       </c>
@@ -8524,7 +8524,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="358" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="4" t="s">
         <v>442</v>
       </c>
@@ -8535,7 +8535,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="359" spans="1:3" ht="36.450000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:3" ht="36.4" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="4" t="s">
         <v>442</v>
       </c>
@@ -8546,7 +8546,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="360" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="4" t="s">
         <v>442</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="361" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="4" t="s">
         <v>442</v>
       </c>
@@ -8568,7 +8568,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="362" spans="1:3" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:3" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="4" t="s">
         <v>442</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="363" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="4" t="s">
         <v>442</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="364" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="4" t="s">
         <v>442</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="365" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="4" t="s">
         <v>442</v>
       </c>
@@ -8612,7 +8612,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="366" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="4" t="s">
         <v>442</v>
       </c>
@@ -8623,7 +8623,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="367" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="4" t="s">
         <v>442</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="368" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="4" t="s">
         <v>442</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="369" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="4" t="s">
         <v>442</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="370" spans="1:3" ht="46.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:3" ht="46.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A370" s="4" t="s">
         <v>442</v>
       </c>
@@ -8667,7 +8667,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="371" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="4" t="s">
         <v>442</v>
       </c>
@@ -8678,7 +8678,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="372" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="4" t="s">
         <v>442</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="373" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="4" t="s">
         <v>442</v>
       </c>
@@ -8700,7 +8700,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="374" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="4" t="s">
         <v>442</v>
       </c>
@@ -8711,7 +8711,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="375" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="4" t="s">
         <v>442</v>
       </c>
@@ -8722,7 +8722,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="376" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="4" t="s">
         <v>442</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="377" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="4" t="s">
         <v>442</v>
       </c>
@@ -8744,7 +8744,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="378" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="4" t="s">
         <v>442</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="379" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="4" t="s">
         <v>442</v>
       </c>
@@ -8766,7 +8766,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="380" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="4" t="s">
         <v>442</v>
       </c>
@@ -8777,7 +8777,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="381" spans="1:3" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:3" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="4" t="s">
         <v>442</v>
       </c>
@@ -8788,7 +8788,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="382" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="4" t="s">
         <v>442</v>
       </c>
@@ -8799,7 +8799,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="383" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="4" t="s">
         <v>442</v>
       </c>
@@ -8810,7 +8810,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="384" spans="1:3" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:3" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="4" t="s">
         <v>442</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="385" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="6" t="s">
         <v>442</v>
       </c>
@@ -8832,7 +8832,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="386" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="4" t="s">
         <v>442</v>
       </c>
@@ -8843,7 +8843,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="387" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="4" t="s">
         <v>442</v>
       </c>
@@ -8854,7 +8854,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="388" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="4" t="s">
         <v>442</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="389" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="4" t="s">
         <v>442</v>
       </c>
@@ -8876,7 +8876,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="390" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="4" t="s">
         <v>442</v>
       </c>
@@ -8887,7 +8887,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="391" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="4" t="s">
         <v>442</v>
       </c>
@@ -8898,7 +8898,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="392" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="4" t="s">
         <v>442</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="393" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="4" t="s">
         <v>442</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="394" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="4" t="s">
         <v>442</v>
       </c>
@@ -8931,7 +8931,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="395" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="4" t="s">
         <v>442</v>
       </c>
@@ -8942,7 +8942,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="396" spans="1:3" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:3" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="4" t="s">
         <v>442</v>
       </c>
@@ -8953,7 +8953,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="397" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="4" t="s">
         <v>442</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="398" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="4" t="s">
         <v>442</v>
       </c>
@@ -8975,7 +8975,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="399" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="4" t="s">
         <v>442</v>
       </c>
@@ -8986,7 +8986,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="400" spans="1:3" ht="59.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:3" ht="59.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="4" t="s">
         <v>442</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="401" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="6" t="s">
         <v>442</v>
       </c>
@@ -9008,7 +9008,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="402" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="4" t="s">
         <v>442</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="403" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="4" t="s">
         <v>442</v>
       </c>
@@ -9030,7 +9030,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="404" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="4" t="s">
         <v>442</v>
       </c>
@@ -9041,7 +9041,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="405" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="4" t="s">
         <v>442</v>
       </c>
@@ -9052,7 +9052,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="406" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="4" t="s">
         <v>442</v>
       </c>
@@ -9063,7 +9063,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="407" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="4" t="s">
         <v>442</v>
       </c>
@@ -9074,7 +9074,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="408" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="4" t="s">
         <v>442</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="409" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="4" t="s">
         <v>442</v>
       </c>
@@ -9096,7 +9096,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="410" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="4" t="s">
         <v>442</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="411" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" s="4" t="s">
         <v>442</v>
       </c>
@@ -9118,7 +9118,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="4" t="s">
         <v>442</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="6" t="s">
         <v>442</v>
       </c>
@@ -9140,7 +9140,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="6" t="s">
         <v>442</v>
       </c>
@@ -9151,7 +9151,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="415" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="6" t="s">
         <v>442</v>
       </c>
@@ -9162,7 +9162,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="416" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="6" t="s">
         <v>442</v>
       </c>
@@ -9173,7 +9173,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="417" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="6" t="s">
         <v>442</v>
       </c>
@@ -9184,7 +9184,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="418" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="6" t="s">
         <v>442</v>
       </c>
@@ -9195,7 +9195,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="419" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" s="6" t="s">
         <v>442</v>
       </c>
@@ -9206,7 +9206,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="420" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="6" t="s">
         <v>442</v>
       </c>
@@ -9217,7 +9217,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="421" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="4" t="s">
         <v>442</v>
       </c>
@@ -9228,7 +9228,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="422" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="4" t="s">
         <v>442</v>
       </c>
@@ -9239,7 +9239,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="423" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="4" t="s">
         <v>442</v>
       </c>
@@ -9250,7 +9250,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="424" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A424" s="6" t="s">
         <v>835</v>
       </c>
@@ -9264,7 +9264,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425" s="4" t="s">
         <v>835</v>
       </c>
@@ -9278,7 +9278,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A426" s="4" t="s">
         <v>835</v>
       </c>
@@ -9292,7 +9292,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427" s="4" t="s">
         <v>835</v>
       </c>
@@ -9309,7 +9309,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428" s="4" t="s">
         <v>835</v>
       </c>
@@ -9323,7 +9323,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A429" s="4" t="s">
         <v>835</v>
       </c>
@@ -9337,7 +9337,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="430" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A430" s="4" t="s">
         <v>835</v>
       </c>
@@ -9351,7 +9351,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431" s="4" t="s">
         <v>835</v>
       </c>
@@ -9365,7 +9365,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432" s="4" t="s">
         <v>835</v>
       </c>
@@ -9379,7 +9379,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A433" s="4" t="s">
         <v>835</v>
       </c>
@@ -9396,7 +9396,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A434" s="4" t="s">
         <v>835</v>
       </c>
@@ -9413,7 +9413,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A435" s="4" t="s">
         <v>835</v>
       </c>
@@ -9427,7 +9427,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="436" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A436" s="4" t="s">
         <v>835</v>
       </c>
@@ -9441,7 +9441,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A437" s="4" t="s">
         <v>835</v>
       </c>
@@ -9455,7 +9455,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="438" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A438" s="4" t="s">
         <v>835</v>
       </c>
@@ -9469,7 +9469,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="439" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A439" s="4" t="s">
         <v>835</v>
       </c>
@@ -9483,7 +9483,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="440" spans="1:5" ht="60.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:5" ht="60.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A440" s="4" t="s">
         <v>835</v>
       </c>
@@ -9497,7 +9497,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A441" s="4" t="s">
         <v>835</v>
       </c>
@@ -9514,7 +9514,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="442" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A442" s="4" t="s">
         <v>835</v>
       </c>
@@ -9528,7 +9528,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A443" s="4" t="s">
         <v>835</v>
       </c>
@@ -9542,7 +9542,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A444" s="4" t="s">
         <v>835</v>
       </c>
@@ -9556,7 +9556,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A445" s="4" t="s">
         <v>835</v>
       </c>
@@ -9570,7 +9570,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="446" spans="1:5" s="9" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:5" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A446" s="6" t="s">
         <v>835</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A447" s="4" t="s">
         <v>835</v>
       </c>
@@ -9598,7 +9598,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="448" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A448" s="4" t="s">
         <v>835</v>
       </c>
@@ -9612,7 +9612,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="449" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A449" s="4" t="s">
         <v>835</v>
       </c>
@@ -9626,7 +9626,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="450" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A450" s="4" t="s">
         <v>835</v>
       </c>
@@ -9640,7 +9640,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="451" spans="1:5" ht="45.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:5" ht="45.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A451" s="4" t="s">
         <v>835</v>
       </c>
@@ -9654,7 +9654,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="452" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A452" s="6" t="s">
         <v>892</v>
       </c>
@@ -9668,7 +9668,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="453" spans="1:5" s="9" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:5" s="9" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A453" s="6" t="s">
         <v>892</v>
       </c>
@@ -9682,7 +9682,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="454" spans="1:5" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:5" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A454" s="6" t="s">
         <v>892</v>
       </c>
@@ -9696,7 +9696,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="455" spans="1:5" s="9" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:5" s="9" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A455" s="6" t="s">
         <v>892</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="456" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A456" s="6" t="s">
         <v>892</v>
       </c>
@@ -9724,7 +9724,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="457" spans="1:5" s="9" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:5" s="9" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A457" s="6" t="s">
         <v>892</v>
       </c>
@@ -9738,7 +9738,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="458" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A458" s="6" t="s">
         <v>892</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="459" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A459" s="6" t="s">
         <v>892</v>
       </c>
@@ -9766,7 +9766,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="460" spans="1:5" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:5" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A460" s="6" t="s">
         <v>892</v>
       </c>
@@ -9780,7 +9780,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="461" spans="1:5" ht="23.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:5" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A461" s="6" t="s">
         <v>892</v>
       </c>
@@ -9794,7 +9794,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="462" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A462" s="6" t="s">
         <v>892</v>
       </c>
@@ -9808,7 +9808,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="463" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A463" s="6" t="s">
         <v>892</v>
       </c>
@@ -9825,7 +9825,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="464" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A464" s="6" t="s">
         <v>892</v>
       </c>
@@ -9842,7 +9842,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="465" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" s="4" t="s">
         <v>442</v>
       </c>
@@ -9853,7 +9853,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="466" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A466" s="4" t="s">
         <v>7</v>
       </c>
@@ -10096,49 +10096,49 @@
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" customWidth="1"/>
-    <col min="5" max="5" width="59.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="17" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="17"/>
     </row>
-    <row r="4" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="21" t="s">
         <v>952</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>975</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>960</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>961</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>966</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>935</v>
       </c>
@@ -10155,7 +10155,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>934</v>
       </c>
@@ -10172,7 +10172,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>936</v>
       </c>
@@ -10189,7 +10189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>937</v>
       </c>
@@ -10206,7 +10206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>938</v>
       </c>
@@ -10223,7 +10223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>939</v>
       </c>
@@ -10240,7 +10240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>940</v>
       </c>
@@ -10257,22 +10257,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="21" t="s">
         <v>962</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="22" t="s">
         <v>964</v>
       </c>
@@ -10283,7 +10283,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>1</v>
       </c>
@@ -10294,7 +10294,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>2</v>
       </c>
@@ -10305,7 +10305,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>3</v>
       </c>
@@ -10316,7 +10316,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>4</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>5</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>6</v>
       </c>
@@ -10349,7 +10349,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>7</v>
       </c>
@@ -10360,7 +10360,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>8</v>
       </c>
@@ -10371,7 +10371,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>9</v>
       </c>
@@ -10382,37 +10382,37 @@
         <v>953</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>977</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>978</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>991</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>935</v>
       </c>
@@ -10423,7 +10423,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>969</v>
       </c>
@@ -10431,7 +10431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>968</v>
       </c>
@@ -10442,7 +10442,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>972</v>
       </c>
@@ -10453,12 +10453,12 @@
         <v>971</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="21" t="s">
         <v>992</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>998</v>
       </c>
@@ -10466,7 +10466,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>993</v>
       </c>
@@ -10474,7 +10474,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>997</v>
       </c>

</xml_diff>

<commit_message>
correction for PolDed6All fields (#865)
</commit_message>
<xml_diff>
--- a/docs/OED_financial_terms_supported.xlsx
+++ b/docs/OED_financial_terms_supported.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\joh\Joh\07 Dev\OED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joh\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA16F4F-4325-4B39-AD4C-0AF24D71FF8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810C6BD3-C388-4D7B-B487-4BF4FF49DCCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
+    <workbookView xWindow="5220" yWindow="2430" windowWidth="21600" windowHeight="11385" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -3622,26 +3622,26 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="17" t="s">
         <v>924</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>985</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>930</v>
       </c>
@@ -3655,12 +3655,12 @@
         <v>932</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
         <v>926</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F10" s="18" t="s">
         <v>0</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" s="18" t="s">
         <v>1</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" s="18" t="s">
         <v>2</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" s="18" t="s">
         <v>911</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" s="18" t="s">
         <v>912</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
         <v>979</v>
       </c>
@@ -3733,20 +3733,20 @@
   <dimension ref="A1:E466"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <pane ySplit="1" topLeftCell="A424" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D200" sqref="D200:D203"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="68.77734375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="24" style="16" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="9" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -3850,7 +3850,7 @@
       </c>
       <c r="D8" s="16"/>
     </row>
-    <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>7</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>7</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>7</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>7</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>7</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>7</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>7</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>7</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>7</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>7</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>7</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>7</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>7</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>7</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>7</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>7</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>7</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>7</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>7</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>7</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>7</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>7</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>7</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>7</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>7</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>7</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>7</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>7</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>7</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>7</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>7</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>7</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>7</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>7</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>7</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>7</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>7</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>7</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>7</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>7</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>7</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>7</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>7</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>7</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>7</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>7</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>7</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>7</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>7</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>7</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>7</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>7</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>7</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>7</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>7</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>7</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>7</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>7</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>7</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>7</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>7</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>7</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>7</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>7</v>
       </c>
@@ -5238,7 +5238,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>7</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>7</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>7</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>7</v>
       </c>
@@ -5305,10 +5305,10 @@
         <v>229</v>
       </c>
       <c r="D113" s="16" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>7</v>
       </c>
@@ -5319,10 +5319,10 @@
         <v>231</v>
       </c>
       <c r="D114" s="16" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>7</v>
       </c>
@@ -5333,10 +5333,10 @@
         <v>233</v>
       </c>
       <c r="D115" s="16" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>7</v>
       </c>
@@ -5347,10 +5347,10 @@
         <v>235</v>
       </c>
       <c r="D116" s="16" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>7</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>7</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>7</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>7</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>7</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>7</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>7</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>7</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>7</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>7</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>7</v>
       </c>
@@ -5504,7 +5504,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>7</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>7</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>7</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>7</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>7</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>7</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>7</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>7</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>7</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>7</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>7</v>
       </c>
@@ -5658,7 +5658,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>7</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>7</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>7</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>7</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>7</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>7</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>7</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>7</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>7</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>7</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>7</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>7</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>7</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>7</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>7</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>7</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" ht="42.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>7</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="59.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>7</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>7</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>7</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>7</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>7</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>7</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>7</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>7</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>7</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>7</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>7</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>7</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>7</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>7</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>7</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>7</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>7</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>7</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>7</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>7</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>7</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>7</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
         <v>7</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
         <v>7</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
         <v>7</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
         <v>7</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
         <v>7</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
         <v>7</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
         <v>7</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
         <v>7</v>
       </c>
@@ -6301,7 +6301,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
         <v>7</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
         <v>7</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
         <v>7</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
         <v>7</v>
       </c>
@@ -6357,7 +6357,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
         <v>7</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
         <v>7</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
         <v>7</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
         <v>7</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
         <v>7</v>
       </c>
@@ -6427,7 +6427,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
         <v>7</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
         <v>7</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
         <v>7</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
         <v>7</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
         <v>7</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
         <v>7</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
         <v>7</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
         <v>7</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
         <v>7</v>
       </c>
@@ -6562,7 +6562,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
         <v>7</v>
       </c>
@@ -6576,7 +6576,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
         <v>7</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
         <v>7</v>
       </c>
@@ -6604,7 +6604,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
         <v>7</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>7</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
         <v>7</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
         <v>7</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
         <v>7</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
         <v>7</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>7</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
         <v>7</v>
       </c>
@@ -6716,7 +6716,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
         <v>7</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>7</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
         <v>7</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
         <v>7</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
         <v>7</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
         <v>7</v>
       </c>
@@ -6800,7 +6800,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
         <v>7</v>
       </c>
@@ -6817,7 +6817,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
         <v>442</v>
       </c>
@@ -6828,7 +6828,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
         <v>442</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
         <v>442</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
         <v>442</v>
       </c>
@@ -6861,7 +6861,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
         <v>442</v>
       </c>
@@ -6872,7 +6872,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="4" t="s">
         <v>442</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="4" t="s">
         <v>442</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="229" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="4" t="s">
         <v>442</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="4" t="s">
         <v>442</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="4" t="s">
         <v>442</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="232" spans="1:4" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="6" t="s">
         <v>442</v>
       </c>
@@ -6939,7 +6939,7 @@
       </c>
       <c r="D232" s="16"/>
     </row>
-    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="4" t="s">
         <v>442</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="4" t="s">
         <v>442</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="4" t="s">
         <v>442</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="4" t="s">
         <v>442</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="4" t="s">
         <v>442</v>
       </c>
@@ -6994,7 +6994,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="4" t="s">
         <v>442</v>
       </c>
@@ -7005,7 +7005,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="4" t="s">
         <v>442</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="4" t="s">
         <v>442</v>
       </c>
@@ -7027,7 +7027,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="241" spans="1:3" ht="78" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3" ht="78" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="4" t="s">
         <v>442</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="4" t="s">
         <v>442</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="78.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:3" ht="78.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="4" t="s">
         <v>442</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="4" t="s">
         <v>442</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="74.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:3" ht="74.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="4" t="s">
         <v>442</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
         <v>442</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:3" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="4" t="s">
         <v>442</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="4" t="s">
         <v>442</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:3" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="4" t="s">
         <v>442</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="4" t="s">
         <v>442</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="49.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:3" ht="49.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="4" t="s">
         <v>442</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="252" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="4" t="s">
         <v>442</v>
       </c>
@@ -7159,7 +7159,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="253" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="4" t="s">
         <v>442</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
         <v>442</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="4" t="s">
         <v>442</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="4" t="s">
         <v>442</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="257" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="4" t="s">
         <v>442</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="258" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="4" t="s">
         <v>442</v>
       </c>
@@ -7225,7 +7225,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="4" t="s">
         <v>442</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="4" t="s">
         <v>442</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="261" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="4" t="s">
         <v>442</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="4" t="s">
         <v>442</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="263" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
         <v>442</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="264" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="4" t="s">
         <v>442</v>
       </c>
@@ -7291,7 +7291,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="265" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="4" t="s">
         <v>442</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="4" t="s">
         <v>442</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="4" t="s">
         <v>442</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="4" t="s">
         <v>442</v>
       </c>
@@ -7335,7 +7335,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="6" t="s">
         <v>442</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="6" t="s">
         <v>442</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="4" t="s">
         <v>442</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="4" t="s">
         <v>442</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="273" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A273" s="4" t="s">
         <v>442</v>
       </c>
@@ -7405,7 +7405,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="4" t="s">
         <v>442</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="4" t="s">
         <v>442</v>
       </c>
@@ -7436,7 +7436,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="276" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A276" s="4" t="s">
         <v>442</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="4" t="s">
         <v>442</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="6" t="s">
         <v>442</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="6" t="s">
         <v>442</v>
       </c>
@@ -7495,7 +7495,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="6" t="s">
         <v>442</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="6" t="s">
         <v>442</v>
       </c>
@@ -7523,7 +7523,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" s="6" t="s">
         <v>442</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="283" spans="1:5" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="6" t="s">
         <v>442</v>
       </c>
@@ -7551,7 +7551,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="284" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
         <v>442</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="285" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="4" t="s">
         <v>442</v>
       </c>
@@ -7576,7 +7576,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="286" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A286" s="4" t="s">
         <v>442</v>
       </c>
@@ -7590,7 +7590,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="4" t="s">
         <v>442</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="4" t="s">
         <v>442</v>
       </c>
@@ -7618,7 +7618,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="4" t="s">
         <v>442</v>
       </c>
@@ -7632,7 +7632,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="4" t="s">
         <v>442</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="4" t="s">
         <v>442</v>
       </c>
@@ -7660,7 +7660,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="4" t="s">
         <v>442</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="4" t="s">
         <v>442</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="4" t="s">
         <v>442</v>
       </c>
@@ -7702,7 +7702,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="4" t="s">
         <v>442</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="4" t="s">
         <v>442</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="4" t="s">
         <v>442</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="4" t="s">
         <v>442</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="4" t="s">
         <v>442</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="4" t="s">
         <v>442</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="4" t="s">
         <v>442</v>
       </c>
@@ -7800,7 +7800,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="4" t="s">
         <v>442</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="4" t="s">
         <v>442</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="4" t="s">
         <v>442</v>
       </c>
@@ -7842,7 +7842,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="4" t="s">
         <v>442</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="4" t="s">
         <v>442</v>
       </c>
@@ -7870,7 +7870,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="4" t="s">
         <v>442</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" s="4" t="s">
         <v>442</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" s="4" t="s">
         <v>442</v>
       </c>
@@ -7912,7 +7912,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" s="4" t="s">
         <v>442</v>
       </c>
@@ -7926,7 +7926,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" s="4" t="s">
         <v>442</v>
       </c>
@@ -7940,7 +7940,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="4" t="s">
         <v>442</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="4" t="s">
         <v>442</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="4" t="s">
         <v>442</v>
       </c>
@@ -7982,7 +7982,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="4" t="s">
         <v>442</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="4" t="s">
         <v>442</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="4" t="s">
         <v>442</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="4" t="s">
         <v>442</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="4" t="s">
         <v>442</v>
       </c>
@@ -8052,7 +8052,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="4" t="s">
         <v>442</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="4" t="s">
         <v>442</v>
       </c>
@@ -8080,7 +8080,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="4" t="s">
         <v>442</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="4" t="s">
         <v>442</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="4" t="s">
         <v>442</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="4" t="s">
         <v>442</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="4" t="s">
         <v>442</v>
       </c>
@@ -8150,7 +8150,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="4" t="s">
         <v>442</v>
       </c>
@@ -8164,7 +8164,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="4" t="s">
         <v>442</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="4" t="s">
         <v>442</v>
       </c>
@@ -8192,7 +8192,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="4" t="s">
         <v>442</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="4" t="s">
         <v>442</v>
       </c>
@@ -8220,7 +8220,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="4" t="s">
         <v>442</v>
       </c>
@@ -8234,7 +8234,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="4" t="s">
         <v>442</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="4" t="s">
         <v>442</v>
       </c>
@@ -8262,7 +8262,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="4" t="s">
         <v>442</v>
       </c>
@@ -8276,7 +8276,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="6" t="s">
         <v>442</v>
       </c>
@@ -8293,7 +8293,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="337" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="4" t="s">
         <v>442</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="338" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="4" t="s">
         <v>442</v>
       </c>
@@ -8315,7 +8315,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="339" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="4" t="s">
         <v>442</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="340" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="4" t="s">
         <v>442</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="341" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="4" t="s">
         <v>442</v>
       </c>
@@ -8348,7 +8348,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="342" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="4" t="s">
         <v>442</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="343" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="4" t="s">
         <v>442</v>
       </c>
@@ -8370,7 +8370,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="344" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="4" t="s">
         <v>442</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="345" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="4" t="s">
         <v>442</v>
       </c>
@@ -8392,7 +8392,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="346" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="4" t="s">
         <v>442</v>
       </c>
@@ -8403,7 +8403,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="347" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="4" t="s">
         <v>442</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="348" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="4" t="s">
         <v>442</v>
       </c>
@@ -8425,7 +8425,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="349" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="6" t="s">
         <v>442</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="350" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="6" t="s">
         <v>442</v>
       </c>
@@ -8447,7 +8447,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="351" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="6" t="s">
         <v>442</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="352" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="6" t="s">
         <v>442</v>
       </c>
@@ -8469,7 +8469,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="353" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="4" t="s">
         <v>442</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="354" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="4" t="s">
         <v>442</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="355" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="4" t="s">
         <v>442</v>
       </c>
@@ -8502,7 +8502,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="356" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="4" t="s">
         <v>442</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="357" spans="1:3" ht="42.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:3" ht="42.4" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="4" t="s">
         <v>442</v>
       </c>
@@ -8524,7 +8524,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="358" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="4" t="s">
         <v>442</v>
       </c>
@@ -8535,7 +8535,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="359" spans="1:3" ht="36.450000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:3" ht="36.4" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="4" t="s">
         <v>442</v>
       </c>
@@ -8546,7 +8546,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="360" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="4" t="s">
         <v>442</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="361" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="4" t="s">
         <v>442</v>
       </c>
@@ -8568,7 +8568,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="362" spans="1:3" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:3" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="4" t="s">
         <v>442</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="363" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="4" t="s">
         <v>442</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="364" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="4" t="s">
         <v>442</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="365" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="4" t="s">
         <v>442</v>
       </c>
@@ -8612,7 +8612,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="366" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="4" t="s">
         <v>442</v>
       </c>
@@ -8623,7 +8623,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="367" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="4" t="s">
         <v>442</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="368" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="4" t="s">
         <v>442</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="369" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="4" t="s">
         <v>442</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="370" spans="1:3" ht="46.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:3" ht="46.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A370" s="4" t="s">
         <v>442</v>
       </c>
@@ -8667,7 +8667,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="371" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="4" t="s">
         <v>442</v>
       </c>
@@ -8678,7 +8678,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="372" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="4" t="s">
         <v>442</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="373" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="4" t="s">
         <v>442</v>
       </c>
@@ -8700,7 +8700,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="374" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="4" t="s">
         <v>442</v>
       </c>
@@ -8711,7 +8711,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="375" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="4" t="s">
         <v>442</v>
       </c>
@@ -8722,7 +8722,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="376" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="4" t="s">
         <v>442</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="377" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="4" t="s">
         <v>442</v>
       </c>
@@ -8744,7 +8744,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="378" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="4" t="s">
         <v>442</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="379" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="4" t="s">
         <v>442</v>
       </c>
@@ -8766,7 +8766,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="380" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="4" t="s">
         <v>442</v>
       </c>
@@ -8777,7 +8777,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="381" spans="1:3" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:3" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="4" t="s">
         <v>442</v>
       </c>
@@ -8788,7 +8788,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="382" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="4" t="s">
         <v>442</v>
       </c>
@@ -8799,7 +8799,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="383" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="4" t="s">
         <v>442</v>
       </c>
@@ -8810,7 +8810,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="384" spans="1:3" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:3" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="4" t="s">
         <v>442</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="385" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="6" t="s">
         <v>442</v>
       </c>
@@ -8832,7 +8832,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="386" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="4" t="s">
         <v>442</v>
       </c>
@@ -8843,7 +8843,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="387" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="4" t="s">
         <v>442</v>
       </c>
@@ -8854,7 +8854,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="388" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="4" t="s">
         <v>442</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="389" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="4" t="s">
         <v>442</v>
       </c>
@@ -8876,7 +8876,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="390" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="4" t="s">
         <v>442</v>
       </c>
@@ -8887,7 +8887,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="391" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="4" t="s">
         <v>442</v>
       </c>
@@ -8898,7 +8898,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="392" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="4" t="s">
         <v>442</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="393" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="4" t="s">
         <v>442</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="394" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="4" t="s">
         <v>442</v>
       </c>
@@ -8931,7 +8931,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="395" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="4" t="s">
         <v>442</v>
       </c>
@@ -8942,7 +8942,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="396" spans="1:3" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:3" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="4" t="s">
         <v>442</v>
       </c>
@@ -8953,7 +8953,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="397" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="4" t="s">
         <v>442</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="398" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="4" t="s">
         <v>442</v>
       </c>
@@ -8975,7 +8975,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="399" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="4" t="s">
         <v>442</v>
       </c>
@@ -8986,7 +8986,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="400" spans="1:3" ht="59.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:3" ht="59.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="4" t="s">
         <v>442</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="401" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="6" t="s">
         <v>442</v>
       </c>
@@ -9008,7 +9008,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="402" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="4" t="s">
         <v>442</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="403" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="4" t="s">
         <v>442</v>
       </c>
@@ -9030,7 +9030,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="404" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="4" t="s">
         <v>442</v>
       </c>
@@ -9041,7 +9041,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="405" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="4" t="s">
         <v>442</v>
       </c>
@@ -9052,7 +9052,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="406" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="4" t="s">
         <v>442</v>
       </c>
@@ -9063,7 +9063,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="407" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="4" t="s">
         <v>442</v>
       </c>
@@ -9074,7 +9074,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="408" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="4" t="s">
         <v>442</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="409" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="4" t="s">
         <v>442</v>
       </c>
@@ -9096,7 +9096,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="410" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="4" t="s">
         <v>442</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="411" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" s="4" t="s">
         <v>442</v>
       </c>
@@ -9118,7 +9118,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="4" t="s">
         <v>442</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="6" t="s">
         <v>442</v>
       </c>
@@ -9140,7 +9140,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="6" t="s">
         <v>442</v>
       </c>
@@ -9151,7 +9151,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="415" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="6" t="s">
         <v>442</v>
       </c>
@@ -9162,7 +9162,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="416" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="6" t="s">
         <v>442</v>
       </c>
@@ -9173,7 +9173,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="417" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="6" t="s">
         <v>442</v>
       </c>
@@ -9184,7 +9184,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="418" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="6" t="s">
         <v>442</v>
       </c>
@@ -9195,7 +9195,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="419" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" s="6" t="s">
         <v>442</v>
       </c>
@@ -9206,7 +9206,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="420" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="6" t="s">
         <v>442</v>
       </c>
@@ -9217,7 +9217,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="421" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="4" t="s">
         <v>442</v>
       </c>
@@ -9228,7 +9228,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="422" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="4" t="s">
         <v>442</v>
       </c>
@@ -9239,7 +9239,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="423" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="4" t="s">
         <v>442</v>
       </c>
@@ -9250,7 +9250,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="424" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A424" s="6" t="s">
         <v>835</v>
       </c>
@@ -9264,7 +9264,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425" s="4" t="s">
         <v>835</v>
       </c>
@@ -9278,7 +9278,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A426" s="4" t="s">
         <v>835</v>
       </c>
@@ -9292,7 +9292,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427" s="4" t="s">
         <v>835</v>
       </c>
@@ -9309,7 +9309,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428" s="4" t="s">
         <v>835</v>
       </c>
@@ -9323,7 +9323,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A429" s="4" t="s">
         <v>835</v>
       </c>
@@ -9337,7 +9337,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="430" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A430" s="4" t="s">
         <v>835</v>
       </c>
@@ -9351,7 +9351,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431" s="4" t="s">
         <v>835</v>
       </c>
@@ -9365,7 +9365,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432" s="4" t="s">
         <v>835</v>
       </c>
@@ -9379,7 +9379,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A433" s="4" t="s">
         <v>835</v>
       </c>
@@ -9396,7 +9396,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A434" s="4" t="s">
         <v>835</v>
       </c>
@@ -9413,7 +9413,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A435" s="4" t="s">
         <v>835</v>
       </c>
@@ -9427,7 +9427,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="436" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A436" s="4" t="s">
         <v>835</v>
       </c>
@@ -9441,7 +9441,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A437" s="4" t="s">
         <v>835</v>
       </c>
@@ -9455,7 +9455,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="438" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A438" s="4" t="s">
         <v>835</v>
       </c>
@@ -9469,7 +9469,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="439" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A439" s="4" t="s">
         <v>835</v>
       </c>
@@ -9483,7 +9483,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="440" spans="1:5" ht="60.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:5" ht="60.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A440" s="4" t="s">
         <v>835</v>
       </c>
@@ -9497,7 +9497,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A441" s="4" t="s">
         <v>835</v>
       </c>
@@ -9514,7 +9514,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="442" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A442" s="4" t="s">
         <v>835</v>
       </c>
@@ -9528,7 +9528,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A443" s="4" t="s">
         <v>835</v>
       </c>
@@ -9542,7 +9542,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A444" s="4" t="s">
         <v>835</v>
       </c>
@@ -9556,7 +9556,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A445" s="4" t="s">
         <v>835</v>
       </c>
@@ -9570,7 +9570,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="446" spans="1:5" s="9" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:5" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A446" s="6" t="s">
         <v>835</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A447" s="4" t="s">
         <v>835</v>
       </c>
@@ -9598,7 +9598,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="448" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A448" s="4" t="s">
         <v>835</v>
       </c>
@@ -9612,7 +9612,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="449" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A449" s="4" t="s">
         <v>835</v>
       </c>
@@ -9626,7 +9626,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="450" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A450" s="4" t="s">
         <v>835</v>
       </c>
@@ -9640,7 +9640,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="451" spans="1:5" ht="45.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:5" ht="45.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A451" s="4" t="s">
         <v>835</v>
       </c>
@@ -9654,7 +9654,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="452" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A452" s="6" t="s">
         <v>892</v>
       </c>
@@ -9668,7 +9668,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="453" spans="1:5" s="9" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:5" s="9" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A453" s="6" t="s">
         <v>892</v>
       </c>
@@ -9682,7 +9682,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="454" spans="1:5" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:5" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A454" s="6" t="s">
         <v>892</v>
       </c>
@@ -9696,7 +9696,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="455" spans="1:5" s="9" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:5" s="9" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A455" s="6" t="s">
         <v>892</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="456" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A456" s="6" t="s">
         <v>892</v>
       </c>
@@ -9724,7 +9724,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="457" spans="1:5" s="9" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:5" s="9" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A457" s="6" t="s">
         <v>892</v>
       </c>
@@ -9738,7 +9738,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="458" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A458" s="6" t="s">
         <v>892</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="459" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A459" s="6" t="s">
         <v>892</v>
       </c>
@@ -9766,7 +9766,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="460" spans="1:5" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:5" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A460" s="6" t="s">
         <v>892</v>
       </c>
@@ -9780,7 +9780,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="461" spans="1:5" ht="23.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:5" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A461" s="6" t="s">
         <v>892</v>
       </c>
@@ -9794,7 +9794,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="462" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A462" s="6" t="s">
         <v>892</v>
       </c>
@@ -9808,7 +9808,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="463" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A463" s="6" t="s">
         <v>892</v>
       </c>
@@ -9825,7 +9825,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="464" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A464" s="6" t="s">
         <v>892</v>
       </c>
@@ -9842,7 +9842,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="465" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" s="4" t="s">
         <v>442</v>
       </c>
@@ -9853,7 +9853,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="466" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A466" s="4" t="s">
         <v>7</v>
       </c>
@@ -10096,49 +10096,49 @@
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" customWidth="1"/>
-    <col min="5" max="5" width="59.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="17" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="17"/>
     </row>
-    <row r="4" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="21" t="s">
         <v>952</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>975</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>960</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>961</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>966</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>935</v>
       </c>
@@ -10155,7 +10155,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>934</v>
       </c>
@@ -10172,7 +10172,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>936</v>
       </c>
@@ -10189,7 +10189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>937</v>
       </c>
@@ -10206,7 +10206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>938</v>
       </c>
@@ -10223,7 +10223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>939</v>
       </c>
@@ -10240,7 +10240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>940</v>
       </c>
@@ -10257,22 +10257,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="21" t="s">
         <v>962</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="22" t="s">
         <v>964</v>
       </c>
@@ -10283,7 +10283,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>1</v>
       </c>
@@ -10294,7 +10294,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>2</v>
       </c>
@@ -10305,7 +10305,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>3</v>
       </c>
@@ -10316,7 +10316,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>4</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>5</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>6</v>
       </c>
@@ -10349,7 +10349,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>7</v>
       </c>
@@ -10360,7 +10360,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>8</v>
       </c>
@@ -10371,7 +10371,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>9</v>
       </c>
@@ -10382,37 +10382,37 @@
         <v>953</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>977</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>978</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>991</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>935</v>
       </c>
@@ -10423,7 +10423,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>969</v>
       </c>
@@ -10431,7 +10431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>968</v>
       </c>
@@ -10442,7 +10442,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>972</v>
       </c>
@@ -10453,12 +10453,12 @@
         <v>971</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="21" t="s">
         <v>992</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>998</v>
       </c>
@@ -10466,7 +10466,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>993</v>
       </c>
@@ -10474,7 +10474,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>997</v>
       </c>

</xml_diff>

<commit_message>
no support for Cond Cov1-5 yet
</commit_message>
<xml_diff>
--- a/docs/OED_financial_terms_supported.xlsx
+++ b/docs/OED_financial_terms_supported.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\joh\dev\OasisLMF_backallocation2\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_backallocation2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55032CE-ED11-4615-924C-250D5815B582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BD5F59-DB1F-499E-B7EB-3A613DE845D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
+    <workbookView xWindow="25507" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="1001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="1000">
   <si>
     <t>File Name</t>
   </si>
@@ -3096,9 +3096,6 @@
   </si>
   <si>
     <t>v1.26</t>
-  </si>
-  <si>
-    <t>1,2,3,4,5,6</t>
   </si>
 </sst>
 </file>
@@ -3628,7 +3625,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3739,8 +3736,8 @@
   <dimension ref="A1:E466"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -6192,7 +6189,7 @@
         <v>349</v>
       </c>
       <c r="D177" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.75">
@@ -6206,7 +6203,7 @@
         <v>351</v>
       </c>
       <c r="D178" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.75">
@@ -6220,7 +6217,7 @@
         <v>353</v>
       </c>
       <c r="D179" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.75">
@@ -6248,7 +6245,7 @@
         <v>357</v>
       </c>
       <c r="D181" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.75">
@@ -6262,7 +6259,7 @@
         <v>359</v>
       </c>
       <c r="D182" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.75">
@@ -6276,7 +6273,7 @@
         <v>361</v>
       </c>
       <c r="D183" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.75">
@@ -6290,7 +6287,7 @@
         <v>363</v>
       </c>
       <c r="D184" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.75">
@@ -6318,7 +6315,7 @@
         <v>367</v>
       </c>
       <c r="D186" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.75">
@@ -6332,7 +6329,7 @@
         <v>369</v>
       </c>
       <c r="D187" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.75">
@@ -6346,7 +6343,7 @@
         <v>371</v>
       </c>
       <c r="D188" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.75">
@@ -6360,7 +6357,7 @@
         <v>373</v>
       </c>
       <c r="D189" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.75">
@@ -6388,7 +6385,7 @@
         <v>377</v>
       </c>
       <c r="D191" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.75">
@@ -6402,7 +6399,7 @@
         <v>379</v>
       </c>
       <c r="D192" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.75">
@@ -6416,7 +6413,7 @@
         <v>381</v>
       </c>
       <c r="D193" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.75">
@@ -6430,7 +6427,7 @@
         <v>383</v>
       </c>
       <c r="D194" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.75">
@@ -6458,7 +6455,7 @@
         <v>387</v>
       </c>
       <c r="D196" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.75">
@@ -6472,7 +6469,7 @@
         <v>389</v>
       </c>
       <c r="D197" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.75">
@@ -6486,7 +6483,7 @@
         <v>391</v>
       </c>
       <c r="D198" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.75">
@@ -6500,7 +6497,7 @@
         <v>393</v>
       </c>
       <c r="D199" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.75">
@@ -6607,7 +6604,7 @@
         <v>407</v>
       </c>
       <c r="D206" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.75">
@@ -6621,7 +6618,7 @@
         <v>409</v>
       </c>
       <c r="D207" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.75">
@@ -6649,7 +6646,7 @@
         <v>413</v>
       </c>
       <c r="D209" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.75">
@@ -6663,7 +6660,7 @@
         <v>415</v>
       </c>
       <c r="D210" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.75">
@@ -6691,7 +6688,7 @@
         <v>419</v>
       </c>
       <c r="D212" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.75">
@@ -6705,7 +6702,7 @@
         <v>421</v>
       </c>
       <c r="D213" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.75">
@@ -6733,7 +6730,7 @@
         <v>425</v>
       </c>
       <c r="D215" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.75">
@@ -6747,7 +6744,7 @@
         <v>427</v>
       </c>
       <c r="D216" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.75">
@@ -6775,7 +6772,7 @@
         <v>431</v>
       </c>
       <c r="D218" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.75">
@@ -6789,7 +6786,7 @@
         <v>433</v>
       </c>
       <c r="D219" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.75">
@@ -10096,10 +10093,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B2:F51"/>
+  <dimension ref="B2:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -10225,8 +10222,8 @@
       <c r="E15" t="s">
         <v>951</v>
       </c>
-      <c r="F15" s="20" t="s">
-        <v>1000</v>
+      <c r="F15" s="20">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.75">
@@ -10243,248 +10240,282 @@
         <v>952</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>1000</v>
+        <v>949</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B17" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C17">
         <v>6</v>
       </c>
       <c r="D17" t="s">
+        <v>937</v>
+      </c>
+      <c r="E17" t="s">
+        <v>952</v>
+      </c>
+      <c r="F17" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.75">
+      <c r="B18" t="s">
+        <v>933</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>937</v>
+      </c>
+      <c r="E18" t="s">
+        <v>952</v>
+      </c>
+      <c r="F18" s="20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.75">
+      <c r="B19" t="s">
+        <v>934</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
         <v>938</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E19" t="s">
         <v>953</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F19" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="18.5" x14ac:dyDescent="0.9">
-      <c r="B19" s="21" t="s">
+    <row r="21" spans="2:6" ht="18.5" x14ac:dyDescent="0.9">
+      <c r="B21" s="21" t="s">
         <v>956</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B21" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.75">
+      <c r="B23" t="s">
         <v>970</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B22" t="s">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.75">
+      <c r="B24" t="s">
         <v>959</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B24" s="22" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.75">
+      <c r="B26" s="22" t="s">
         <v>958</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C26" s="22" t="s">
         <v>939</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D26" s="22" t="s">
         <v>940</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B29">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B30">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B31">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B35">
         <v>9</v>
       </c>
-      <c r="C33">
+      <c r="C35">
         <v>3</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D35" t="s">
         <v>947</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B35" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B36" t="s">
-        <v>968</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B37" t="s">
-        <v>971</v>
+        <v>961</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B38" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B39" t="s">
-        <v>984</v>
+        <v>971</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B40" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B41" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B42" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B42" s="1" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B44" s="1" t="s">
         <v>929</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>935</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D44" s="22" t="s">
         <v>936</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B43" t="s">
-        <v>963</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B44" t="s">
-        <v>962</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B45" t="s">
+        <v>963</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B46" t="s">
+        <v>962</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B47" t="s">
         <v>966</v>
       </c>
-      <c r="C45">
+      <c r="C47">
         <v>3</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="18.5" x14ac:dyDescent="0.9">
-      <c r="B48" s="21" t="s">
+    <row r="50" spans="2:3" ht="18.5" x14ac:dyDescent="0.9">
+      <c r="B50" s="21" t="s">
         <v>985</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.75">
-      <c r="B49" t="s">
-        <v>991</v>
-      </c>
-      <c r="C49" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.75">
-      <c r="B50" t="s">
-        <v>986</v>
-      </c>
-      <c r="C50" t="s">
-        <v>988</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.75">
       <c r="B51" t="s">
+        <v>991</v>
+      </c>
+      <c r="C51" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B52" t="s">
+        <v>986</v>
+      </c>
+      <c r="C52" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B53" t="s">
         <v>990</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C53" t="s">
         <v>989</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more information about supported reinsurance fields for different contract types
</commit_message>
<xml_diff>
--- a/docs/OED_financial_terms_supported.xlsx
+++ b/docs/OED_financial_terms_supported.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_backallocation2\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\joh\dev\OasisLMF_update-fm-docs\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BD5F59-DB1F-499E-B7EB-3A613DE845D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5C6EB2-42D1-49A2-8DE3-189226CB6E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25507" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
+    <workbookView xWindow="28000" yWindow="2400" windowWidth="19200" windowHeight="9900" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="1000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="1014">
   <si>
     <t>File Name</t>
   </si>
@@ -2975,15 +2975,9 @@
     <t>Cycle</t>
   </si>
   <si>
-    <t xml:space="preserve">The terms are applied in the order of processing cycle. The net loss is output from each processing cycle and feeds into the next processing cycle. </t>
-  </si>
-  <si>
     <t>The calculated loss is passed from one level to the next, and the output from the final level is the gross loss.</t>
   </si>
   <si>
-    <t>Within each cycle there are three fixed levels of calculation.</t>
-  </si>
-  <si>
     <t>Risk level</t>
   </si>
   <si>
@@ -2996,27 +2990,12 @@
     <t>OccAttachment, OccLimit, PlacedPercent</t>
   </si>
   <si>
-    <t>Layer level</t>
-  </si>
-  <si>
     <t>The final step is to difference the input and the output, and pass through the net loss to the next processing cycle.</t>
   </si>
   <si>
-    <t>The first level groups losses by location and by policy. The calculation filters losses that are within the scope of each reinsurance layer and passes them through to the next level. All other losses are set to zero.</t>
-  </si>
-  <si>
     <t>All supported direct insurance terms are associated with a fixed 'FM level'. The level specifies how losses should be grouped together for processing.</t>
   </si>
   <si>
-    <t>Each Reinsurance layer (identified by ReinsNumber) is allocated to a processing cycle depending on the InuringPriority and RiskLevel. The number of cycles will vary depending on the data in the ri_info and ri_scope file</t>
-  </si>
-  <si>
-    <t>The second level groups loss to the Risk Level (either location, or policy, or account) and applies the CededPercent and then any risk terms to the losses.</t>
-  </si>
-  <si>
-    <t>The third level groups losses to the Layer level (which means summing losses across all risks in scope of the reinsurance layer) and applies the occurrence terms and finally the PlacedPercent which results in the Reinsurance layer loss</t>
-  </si>
-  <si>
     <t>Order of Operation</t>
   </si>
   <si>
@@ -3050,9 +3029,6 @@
     <t>Is the field supported by the OasisLMF financial module (Yes/No/(blank))</t>
   </si>
   <si>
-    <t>The order of terms appled within each level is determined by a specific calcrule that is invoked by the calculation.</t>
-  </si>
-  <si>
     <t>References</t>
   </si>
   <si>
@@ -3096,6 +3072,132 @@
   </si>
   <si>
     <t>v1.26</t>
+  </si>
+  <si>
+    <t>QS</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>FAC</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>CXL</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Facultative</t>
+  </si>
+  <si>
+    <t>Quota Share</t>
+  </si>
+  <si>
+    <t>Surplus Share</t>
+  </si>
+  <si>
+    <t>Catastrophe Excess of Loss</t>
+  </si>
+  <si>
+    <t>Per Risk Excess of Loss</t>
+  </si>
+  <si>
+    <t>Each Reinsurance contract (identified by ReinsNumber) is allocated to a processing cycle depending on the InuringPriority and RiskLevel. The number of cycles will vary depending on the data in the ri_info and ri_scope file</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x*</t>
+  </si>
+  <si>
+    <t>*Only for Surplus Share is CededPercent specified per risk and taken from the reinsurance scope file. All other reinsurance types use the CededPercent in the reinsurance info file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The contracts are allocated to a processing cycle based on InuringPriority and RiskLevel and processed in cycle order. The net loss is output from each processing cycle and feeds into the next processing cycle. </t>
+  </si>
+  <si>
+    <t>Contract level</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Location Policy Level: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The first level sums losses by location and by policy. The calculation filters losses that are within the scope of each reinsurance layer and passes them through to the next level. All other losses are set to zero because they are outside the scope of the contract.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Risk Level:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The second level sums loss to the Risk Level (either location, or policy, or account) and applies the CededPercent and then any risk terms to the losses.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Contract Level: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The third level groups losses to the contract level (which means summing losses across all risks in scope of the reinsurance layer) and applies the occurrence terms and finally the PlacedPercent which results in the Reinsurance contract loss</t>
+    </r>
+  </si>
+  <si>
+    <t>Within each cycle there are three fixed levels of calculation. Each level involves summing losses and then applying a financial terms calculation.</t>
+  </si>
+  <si>
+    <t>The following types of reinsurance are supported and use the fields in reinsurance info and reinsurance scope files indicated in the matrix</t>
   </si>
 </sst>
 </file>
@@ -3171,7 +3273,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -3179,12 +3281,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3245,6 +3362,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3641,7 +3762,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B4" t="s">
-        <v>978</v>
+        <v>971</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.75">
@@ -3649,13 +3770,13 @@
         <v>925</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>998</v>
+        <v>990</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>926</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>999</v>
+        <v>991</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.75">
@@ -3668,7 +3789,7 @@
         <v>922</v>
       </c>
       <c r="F9" t="s">
-        <v>982</v>
+        <v>975</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.75">
@@ -3692,7 +3813,7 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>981</v>
+        <v>974</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.75">
@@ -3700,7 +3821,7 @@
         <v>908</v>
       </c>
       <c r="G13" t="s">
-        <v>983</v>
+        <v>976</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.75">
@@ -3713,10 +3834,10 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B16" s="25" t="s">
-        <v>973</v>
+        <v>966</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>974</v>
+        <v>967</v>
       </c>
     </row>
   </sheetData>
@@ -3736,8 +3857,8 @@
   <dimension ref="A1:E466"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3766,7 +3887,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -3802,7 +3923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -3827,7 +3948,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -3853,7 +3974,7 @@
       </c>
       <c r="D8" s="16"/>
     </row>
-    <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -3878,7 +3999,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -3961,7 +4082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -3975,10 +4096,10 @@
         <v>910</v>
       </c>
       <c r="E18" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -3992,7 +4113,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
@@ -4006,7 +4127,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -4020,7 +4141,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
@@ -4034,7 +4155,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
@@ -4048,7 +4169,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -4062,7 +4183,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A25" s="4" t="s">
         <v>7</v>
       </c>
@@ -4076,7 +4197,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -4090,7 +4211,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
@@ -4104,7 +4225,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
@@ -4118,7 +4239,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -4132,7 +4253,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A30" s="4" t="s">
         <v>7</v>
       </c>
@@ -4146,7 +4267,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -4160,7 +4281,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A32" s="4" t="s">
         <v>7</v>
       </c>
@@ -4174,7 +4295,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A33" s="4" t="s">
         <v>7</v>
       </c>
@@ -4188,7 +4309,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
@@ -4202,7 +4323,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A35" s="4" t="s">
         <v>7</v>
       </c>
@@ -4216,7 +4337,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A36" s="4" t="s">
         <v>7</v>
       </c>
@@ -4230,7 +4351,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
@@ -4244,7 +4365,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A38" s="4" t="s">
         <v>7</v>
       </c>
@@ -4258,7 +4379,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
@@ -4272,7 +4393,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A40" s="4" t="s">
         <v>7</v>
       </c>
@@ -4286,7 +4407,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A41" s="4" t="s">
         <v>7</v>
       </c>
@@ -4300,7 +4421,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
@@ -4314,7 +4435,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A43" s="4" t="s">
         <v>7</v>
       </c>
@@ -4328,7 +4449,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -4342,7 +4463,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
@@ -4356,7 +4477,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -4370,7 +4491,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -4384,7 +4505,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A48" s="4" t="s">
         <v>7</v>
       </c>
@@ -4398,7 +4519,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
@@ -4412,7 +4533,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A50" s="4" t="s">
         <v>7</v>
       </c>
@@ -4426,7 +4547,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A51" s="4" t="s">
         <v>7</v>
       </c>
@@ -4440,7 +4561,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A52" s="4" t="s">
         <v>7</v>
       </c>
@@ -4454,7 +4575,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A53" s="4" t="s">
         <v>7</v>
       </c>
@@ -4468,7 +4589,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -4482,7 +4603,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A55" s="4" t="s">
         <v>7</v>
       </c>
@@ -4496,7 +4617,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A56" s="4" t="s">
         <v>7</v>
       </c>
@@ -4510,7 +4631,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A57" s="4" t="s">
         <v>7</v>
       </c>
@@ -4524,7 +4645,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A58" s="4" t="s">
         <v>7</v>
       </c>
@@ -4538,7 +4659,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A59" s="4" t="s">
         <v>7</v>
       </c>
@@ -4552,7 +4673,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A60" s="4" t="s">
         <v>7</v>
       </c>
@@ -4566,7 +4687,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A61" s="4" t="s">
         <v>7</v>
       </c>
@@ -4580,7 +4701,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
@@ -4594,7 +4715,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A63" s="4" t="s">
         <v>7</v>
       </c>
@@ -4608,7 +4729,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A64" s="4" t="s">
         <v>7</v>
       </c>
@@ -4622,7 +4743,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A65" s="4" t="s">
         <v>7</v>
       </c>
@@ -4636,7 +4757,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A66" s="4" t="s">
         <v>7</v>
       </c>
@@ -4650,7 +4771,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A67" s="4" t="s">
         <v>7</v>
       </c>
@@ -4664,7 +4785,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A68" s="4" t="s">
         <v>7</v>
       </c>
@@ -4678,7 +4799,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A69" s="4" t="s">
         <v>7</v>
       </c>
@@ -4692,7 +4813,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A70" s="4" t="s">
         <v>7</v>
       </c>
@@ -4750,7 +4871,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:5" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A75" s="6" t="s">
         <v>7</v>
       </c>
@@ -4764,7 +4885,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A76" s="4" t="s">
         <v>7</v>
       </c>
@@ -4781,7 +4902,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A77" s="4" t="s">
         <v>7</v>
       </c>
@@ -4795,7 +4916,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
@@ -4809,7 +4930,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A79" s="4" t="s">
         <v>7</v>
       </c>
@@ -4823,7 +4944,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A80" s="4" t="s">
         <v>7</v>
       </c>
@@ -4837,7 +4958,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A81" s="4" t="s">
         <v>7</v>
       </c>
@@ -4854,7 +4975,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A82" s="4" t="s">
         <v>7</v>
       </c>
@@ -4871,7 +4992,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A83" s="4" t="s">
         <v>7</v>
       </c>
@@ -4888,7 +5009,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A84" s="4" t="s">
         <v>7</v>
       </c>
@@ -4902,7 +5023,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:5" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
       <c r="A85" s="4" t="s">
         <v>7</v>
       </c>
@@ -4916,7 +5037,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
@@ -4930,10 +5051,10 @@
         <v>910</v>
       </c>
       <c r="E86" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.75">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A87" s="4" t="s">
         <v>7</v>
       </c>
@@ -4947,7 +5068,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A88" s="4" t="s">
         <v>7</v>
       </c>
@@ -4961,7 +5082,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A89" s="4" t="s">
         <v>7</v>
       </c>
@@ -4975,7 +5096,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A90" s="4" t="s">
         <v>7</v>
       </c>
@@ -4989,7 +5110,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A91" s="4" t="s">
         <v>7</v>
       </c>
@@ -5003,7 +5124,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A92" s="4" t="s">
         <v>7</v>
       </c>
@@ -5017,7 +5138,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A93" s="4" t="s">
         <v>7</v>
       </c>
@@ -5031,7 +5152,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
@@ -5045,7 +5166,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A95" s="4" t="s">
         <v>7</v>
       </c>
@@ -5059,7 +5180,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A96" s="4" t="s">
         <v>7</v>
       </c>
@@ -5073,7 +5194,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A97" s="4" t="s">
         <v>7</v>
       </c>
@@ -5087,7 +5208,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A98" s="4" t="s">
         <v>7</v>
       </c>
@@ -5101,7 +5222,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A99" s="4" t="s">
         <v>7</v>
       </c>
@@ -5115,7 +5236,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A100" s="4" t="s">
         <v>7</v>
       </c>
@@ -5129,7 +5250,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A101" s="4" t="s">
         <v>7</v>
       </c>
@@ -5143,7 +5264,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
@@ -5157,7 +5278,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A103" s="4" t="s">
         <v>7</v>
       </c>
@@ -5171,7 +5292,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A104" s="4" t="s">
         <v>7</v>
       </c>
@@ -5185,7 +5306,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A105" s="4" t="s">
         <v>7</v>
       </c>
@@ -5199,7 +5320,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A106" s="4" t="s">
         <v>7</v>
       </c>
@@ -5213,7 +5334,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A107" s="4" t="s">
         <v>7</v>
       </c>
@@ -5227,7 +5348,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A108" s="4" t="s">
         <v>7</v>
       </c>
@@ -5241,7 +5362,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A109" s="4" t="s">
         <v>7</v>
       </c>
@@ -5255,7 +5376,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
@@ -5269,7 +5390,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A111" s="4" t="s">
         <v>7</v>
       </c>
@@ -5283,7 +5404,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A112" s="4" t="s">
         <v>7</v>
       </c>
@@ -5297,7 +5418,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A113" s="4" t="s">
         <v>7</v>
       </c>
@@ -5311,7 +5432,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A114" s="4" t="s">
         <v>7</v>
       </c>
@@ -5325,7 +5446,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A115" s="4" t="s">
         <v>7</v>
       </c>
@@ -5339,7 +5460,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A116" s="4" t="s">
         <v>7</v>
       </c>
@@ -5353,7 +5474,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A117" s="4" t="s">
         <v>7</v>
       </c>
@@ -5367,7 +5488,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A118" s="4" t="s">
         <v>7</v>
       </c>
@@ -5395,7 +5516,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A120" s="4" t="s">
         <v>7</v>
       </c>
@@ -5409,7 +5530,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A121" s="4" t="s">
         <v>7</v>
       </c>
@@ -5423,7 +5544,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A122" s="4" t="s">
         <v>7</v>
       </c>
@@ -5437,7 +5558,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A123" s="4" t="s">
         <v>7</v>
       </c>
@@ -5451,7 +5572,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A124" s="4" t="s">
         <v>7</v>
       </c>
@@ -5465,7 +5586,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A125" s="4" t="s">
         <v>7</v>
       </c>
@@ -5479,7 +5600,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A126" s="4" t="s">
         <v>7</v>
       </c>
@@ -5493,7 +5614,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A127" s="4" t="s">
         <v>7</v>
       </c>
@@ -5507,7 +5628,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A128" s="4" t="s">
         <v>7</v>
       </c>
@@ -5521,7 +5642,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A129" s="4" t="s">
         <v>7</v>
       </c>
@@ -5535,7 +5656,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A130" s="4" t="s">
         <v>7</v>
       </c>
@@ -5549,7 +5670,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A131" s="4" t="s">
         <v>7</v>
       </c>
@@ -5563,7 +5684,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A132" s="4" t="s">
         <v>7</v>
       </c>
@@ -5577,7 +5698,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A133" s="4" t="s">
         <v>7</v>
       </c>
@@ -5591,7 +5712,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A134" s="4" t="s">
         <v>7</v>
       </c>
@@ -5605,7 +5726,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A135" s="4" t="s">
         <v>7</v>
       </c>
@@ -5619,7 +5740,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A136" s="4" t="s">
         <v>7</v>
       </c>
@@ -5633,7 +5754,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A137" s="4" t="s">
         <v>7</v>
       </c>
@@ -5647,7 +5768,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A138" s="4" t="s">
         <v>7</v>
       </c>
@@ -5661,7 +5782,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A139" s="4" t="s">
         <v>7</v>
       </c>
@@ -5675,7 +5796,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A140" s="4" t="s">
         <v>7</v>
       </c>
@@ -5689,7 +5810,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A141" s="4" t="s">
         <v>7</v>
       </c>
@@ -5703,7 +5824,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A142" s="4" t="s">
         <v>7</v>
       </c>
@@ -5717,7 +5838,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A143" s="4" t="s">
         <v>7</v>
       </c>
@@ -5731,7 +5852,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:4" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
       <c r="A144" s="4" t="s">
         <v>7</v>
       </c>
@@ -5745,7 +5866,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A145" s="4" t="s">
         <v>7</v>
       </c>
@@ -5759,7 +5880,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A146" s="4" t="s">
         <v>7</v>
       </c>
@@ -5773,7 +5894,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A147" s="4" t="s">
         <v>7</v>
       </c>
@@ -5787,7 +5908,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A148" s="4" t="s">
         <v>7</v>
       </c>
@@ -5801,7 +5922,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A149" s="4" t="s">
         <v>7</v>
       </c>
@@ -5815,7 +5936,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:4" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
       <c r="A150" s="4" t="s">
         <v>7</v>
       </c>
@@ -5829,7 +5950,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A151" s="4" t="s">
         <v>7</v>
       </c>
@@ -5843,7 +5964,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A152" s="4" t="s">
         <v>7</v>
       </c>
@@ -5857,7 +5978,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A153" s="4" t="s">
         <v>7</v>
       </c>
@@ -5871,7 +5992,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A154" s="4" t="s">
         <v>7</v>
       </c>
@@ -5885,7 +6006,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="42.45" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:4" ht="42.45" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A155" s="4" t="s">
         <v>7</v>
       </c>
@@ -5899,7 +6020,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="59.7" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:4" ht="59.7" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A156" s="4" t="s">
         <v>7</v>
       </c>
@@ -5913,7 +6034,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A157" s="4" t="s">
         <v>7</v>
       </c>
@@ -5927,7 +6048,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:4" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
       <c r="A158" s="4" t="s">
         <v>7</v>
       </c>
@@ -5941,7 +6062,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A159" s="4" t="s">
         <v>7</v>
       </c>
@@ -5955,7 +6076,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="59" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:4" ht="59" hidden="1" x14ac:dyDescent="0.75">
       <c r="A160" s="4" t="s">
         <v>7</v>
       </c>
@@ -5969,7 +6090,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A161" s="4" t="s">
         <v>7</v>
       </c>
@@ -5983,7 +6104,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:5" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
       <c r="A162" s="4" t="s">
         <v>7</v>
       </c>
@@ -5997,7 +6118,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A163" s="4" t="s">
         <v>7</v>
       </c>
@@ -6077,21 +6198,21 @@
         <v>337</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A170" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>993</v>
+        <v>985</v>
       </c>
       <c r="D170" s="16" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="171" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A171" s="4" t="s">
         <v>7</v>
       </c>
@@ -6099,13 +6220,13 @@
         <v>338</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>994</v>
+        <v>986</v>
       </c>
       <c r="D171" s="16" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A172" s="4" t="s">
         <v>7</v>
       </c>
@@ -6113,13 +6234,13 @@
         <v>339</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>995</v>
+        <v>987</v>
       </c>
       <c r="D172" s="16" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="173" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A173" s="4" t="s">
         <v>7</v>
       </c>
@@ -6133,7 +6254,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A174" s="4" t="s">
         <v>7</v>
       </c>
@@ -6147,10 +6268,10 @@
         <v>910</v>
       </c>
       <c r="E174" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.75">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A175" s="4" t="s">
         <v>7</v>
       </c>
@@ -6164,7 +6285,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A176" s="4" t="s">
         <v>7</v>
       </c>
@@ -6178,7 +6299,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A177" s="4" t="s">
         <v>7</v>
       </c>
@@ -6192,7 +6313,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A178" s="4" t="s">
         <v>7</v>
       </c>
@@ -6206,7 +6327,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A179" s="4" t="s">
         <v>7</v>
       </c>
@@ -6220,7 +6341,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A180" s="4" t="s">
         <v>7</v>
       </c>
@@ -6234,7 +6355,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A181" s="4" t="s">
         <v>7</v>
       </c>
@@ -6248,7 +6369,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A182" s="4" t="s">
         <v>7</v>
       </c>
@@ -6262,7 +6383,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A183" s="4" t="s">
         <v>7</v>
       </c>
@@ -6276,7 +6397,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A184" s="4" t="s">
         <v>7</v>
       </c>
@@ -6290,7 +6411,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A185" s="4" t="s">
         <v>7</v>
       </c>
@@ -6304,7 +6425,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A186" s="4" t="s">
         <v>7</v>
       </c>
@@ -6318,7 +6439,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A187" s="4" t="s">
         <v>7</v>
       </c>
@@ -6332,7 +6453,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A188" s="4" t="s">
         <v>7</v>
       </c>
@@ -6346,7 +6467,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A189" s="4" t="s">
         <v>7</v>
       </c>
@@ -6360,7 +6481,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A190" s="4" t="s">
         <v>7</v>
       </c>
@@ -6374,7 +6495,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A191" s="4" t="s">
         <v>7</v>
       </c>
@@ -6388,7 +6509,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A192" s="4" t="s">
         <v>7</v>
       </c>
@@ -6402,7 +6523,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A193" s="4" t="s">
         <v>7</v>
       </c>
@@ -6416,7 +6537,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A194" s="4" t="s">
         <v>7</v>
       </c>
@@ -6430,7 +6551,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A195" s="4" t="s">
         <v>7</v>
       </c>
@@ -6444,7 +6565,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A196" s="4" t="s">
         <v>7</v>
       </c>
@@ -6458,7 +6579,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A197" s="4" t="s">
         <v>7</v>
       </c>
@@ -6472,7 +6593,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A198" s="4" t="s">
         <v>7</v>
       </c>
@@ -6486,7 +6607,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A199" s="4" t="s">
         <v>7</v>
       </c>
@@ -6500,7 +6621,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A200" s="4" t="s">
         <v>7</v>
       </c>
@@ -6514,7 +6635,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A201" s="4" t="s">
         <v>7</v>
       </c>
@@ -6528,7 +6649,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A202" s="4" t="s">
         <v>7</v>
       </c>
@@ -6542,10 +6663,10 @@
         <v>911</v>
       </c>
       <c r="E202" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.75">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A203" s="4" t="s">
         <v>7</v>
       </c>
@@ -6559,10 +6680,10 @@
         <v>911</v>
       </c>
       <c r="E203" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.75">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A204" s="4" t="s">
         <v>7</v>
       </c>
@@ -6576,10 +6697,10 @@
         <v>911</v>
       </c>
       <c r="E204" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.75">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A205" s="4" t="s">
         <v>7</v>
       </c>
@@ -6593,7 +6714,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A206" s="4" t="s">
         <v>7</v>
       </c>
@@ -6607,7 +6728,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A207" s="4" t="s">
         <v>7</v>
       </c>
@@ -6621,7 +6742,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A208" s="4" t="s">
         <v>7</v>
       </c>
@@ -6635,7 +6756,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A209" s="4" t="s">
         <v>7</v>
       </c>
@@ -6649,7 +6770,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A210" s="4" t="s">
         <v>7</v>
       </c>
@@ -6663,7 +6784,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A211" s="4" t="s">
         <v>7</v>
       </c>
@@ -6677,7 +6798,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A212" s="4" t="s">
         <v>7</v>
       </c>
@@ -6691,7 +6812,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A213" s="4" t="s">
         <v>7</v>
       </c>
@@ -6705,7 +6826,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A214" s="4" t="s">
         <v>7</v>
       </c>
@@ -6719,7 +6840,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A215" s="4" t="s">
         <v>7</v>
       </c>
@@ -6733,7 +6854,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A216" s="4" t="s">
         <v>7</v>
       </c>
@@ -6747,7 +6868,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A217" s="4" t="s">
         <v>7</v>
       </c>
@@ -6761,7 +6882,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A218" s="4" t="s">
         <v>7</v>
       </c>
@@ -6775,7 +6896,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A219" s="4" t="s">
         <v>7</v>
       </c>
@@ -6789,7 +6910,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A220" s="4" t="s">
         <v>7</v>
       </c>
@@ -6803,7 +6924,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A221" s="4" t="s">
         <v>7</v>
       </c>
@@ -6817,7 +6938,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A222" s="4" t="s">
         <v>7</v>
       </c>
@@ -6831,7 +6952,7 @@
         <v>911</v>
       </c>
       <c r="E222" t="s">
-        <v>975</v>
+        <v>968</v>
       </c>
     </row>
     <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
@@ -7374,7 +7495,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="272" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A272" s="4" t="s">
         <v>440</v>
       </c>
@@ -7388,10 +7509,10 @@
         <v>911</v>
       </c>
       <c r="E272" t="s">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.75">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A273" s="4" t="s">
         <v>440</v>
       </c>
@@ -7405,7 +7526,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="274" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="274" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A274" s="4" t="s">
         <v>440</v>
       </c>
@@ -7422,7 +7543,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A275" s="4" t="s">
         <v>440</v>
       </c>
@@ -7436,7 +7557,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A276" s="4" t="s">
         <v>440</v>
       </c>
@@ -7453,7 +7574,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="277" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="277" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A277" s="4" t="s">
         <v>440</v>
       </c>
@@ -7467,7 +7588,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A278" s="4" t="s">
         <v>440</v>
       </c>
@@ -7484,7 +7605,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A279" s="6" t="s">
         <v>440</v>
       </c>
@@ -7498,7 +7619,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A280" s="6" t="s">
         <v>440</v>
       </c>
@@ -7512,7 +7633,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A281" s="6" t="s">
         <v>440</v>
       </c>
@@ -7526,7 +7647,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A282" s="6" t="s">
         <v>440</v>
       </c>
@@ -7540,7 +7661,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A283" s="6" t="s">
         <v>440</v>
       </c>
@@ -7554,7 +7675,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="284" spans="1:5" ht="43.95" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="284" spans="1:5" ht="43.95" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A284" s="6" t="s">
         <v>440</v>
       </c>
@@ -7568,7 +7689,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="285" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="285" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A285" s="6" t="s">
         <v>440</v>
       </c>
@@ -7593,7 +7714,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A287" s="4" t="s">
         <v>440</v>
       </c>
@@ -7607,7 +7728,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A288" s="4" t="s">
         <v>440</v>
       </c>
@@ -7621,7 +7742,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="289" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A289" s="4" t="s">
         <v>440</v>
       </c>
@@ -7635,7 +7756,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="290" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A290" s="4" t="s">
         <v>440</v>
       </c>
@@ -7649,7 +7770,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="291" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A291" s="4" t="s">
         <v>440</v>
       </c>
@@ -7663,7 +7784,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="292" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A292" s="4" t="s">
         <v>440</v>
       </c>
@@ -7677,7 +7798,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="293" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A293" s="4" t="s">
         <v>440</v>
       </c>
@@ -7691,7 +7812,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="294" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A294" s="4" t="s">
         <v>440</v>
       </c>
@@ -7705,7 +7826,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="295" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A295" s="4" t="s">
         <v>440</v>
       </c>
@@ -7719,7 +7840,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="296" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A296" s="4" t="s">
         <v>440</v>
       </c>
@@ -7733,7 +7854,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="297" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A297" s="4" t="s">
         <v>440</v>
       </c>
@@ -7747,7 +7868,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="298" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A298" s="4" t="s">
         <v>440</v>
       </c>
@@ -7761,7 +7882,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="299" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A299" s="4" t="s">
         <v>440</v>
       </c>
@@ -7775,7 +7896,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="300" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A300" s="4" t="s">
         <v>440</v>
       </c>
@@ -7789,7 +7910,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="301" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A301" s="4" t="s">
         <v>440</v>
       </c>
@@ -7803,7 +7924,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="302" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A302" s="4" t="s">
         <v>440</v>
       </c>
@@ -7817,7 +7938,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="303" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A303" s="4" t="s">
         <v>440</v>
       </c>
@@ -7831,7 +7952,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="304" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A304" s="4" t="s">
         <v>440</v>
       </c>
@@ -7845,7 +7966,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="305" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A305" s="4" t="s">
         <v>440</v>
       </c>
@@ -7859,7 +7980,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="306" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A306" s="4" t="s">
         <v>440</v>
       </c>
@@ -7873,7 +7994,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="307" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A307" s="4" t="s">
         <v>440</v>
       </c>
@@ -7887,7 +8008,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="308" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A308" s="4" t="s">
         <v>440</v>
       </c>
@@ -7901,7 +8022,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="309" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A309" s="4" t="s">
         <v>440</v>
       </c>
@@ -7915,7 +8036,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="310" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A310" s="4" t="s">
         <v>440</v>
       </c>
@@ -7929,7 +8050,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="311" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A311" s="4" t="s">
         <v>440</v>
       </c>
@@ -7943,7 +8064,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="312" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A312" s="4" t="s">
         <v>440</v>
       </c>
@@ -7957,7 +8078,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="313" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A313" s="4" t="s">
         <v>440</v>
       </c>
@@ -7971,7 +8092,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="314" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A314" s="4" t="s">
         <v>440</v>
       </c>
@@ -7985,7 +8106,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="315" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A315" s="4" t="s">
         <v>440</v>
       </c>
@@ -7999,7 +8120,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="316" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A316" s="4" t="s">
         <v>440</v>
       </c>
@@ -8013,7 +8134,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="317" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A317" s="4" t="s">
         <v>440</v>
       </c>
@@ -8027,7 +8148,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="318" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A318" s="4" t="s">
         <v>440</v>
       </c>
@@ -8041,7 +8162,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="319" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A319" s="4" t="s">
         <v>440</v>
       </c>
@@ -8055,7 +8176,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="320" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A320" s="4" t="s">
         <v>440</v>
       </c>
@@ -8069,7 +8190,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A321" s="4" t="s">
         <v>440</v>
       </c>
@@ -8083,7 +8204,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A322" s="4" t="s">
         <v>440</v>
       </c>
@@ -8097,7 +8218,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A323" s="4" t="s">
         <v>440</v>
       </c>
@@ -8111,7 +8232,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A324" s="4" t="s">
         <v>440</v>
       </c>
@@ -8125,7 +8246,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A325" s="4" t="s">
         <v>440</v>
       </c>
@@ -8139,7 +8260,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A326" s="4" t="s">
         <v>440</v>
       </c>
@@ -8153,7 +8274,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A327" s="4" t="s">
         <v>440</v>
       </c>
@@ -8167,7 +8288,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A328" s="4" t="s">
         <v>440</v>
       </c>
@@ -8181,7 +8302,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A329" s="4" t="s">
         <v>440</v>
       </c>
@@ -8195,7 +8316,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A330" s="4" t="s">
         <v>440</v>
       </c>
@@ -8209,7 +8330,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A331" s="4" t="s">
         <v>440</v>
       </c>
@@ -8223,7 +8344,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A332" s="4" t="s">
         <v>440</v>
       </c>
@@ -8237,7 +8358,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A333" s="4" t="s">
         <v>440</v>
       </c>
@@ -8251,7 +8372,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="334" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A334" s="4" t="s">
         <v>440</v>
       </c>
@@ -8265,7 +8386,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A335" s="4" t="s">
         <v>440</v>
       </c>
@@ -8279,7 +8400,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="336" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A336" s="6" t="s">
         <v>440</v>
       </c>
@@ -8293,7 +8414,7 @@
         <v>910</v>
       </c>
       <c r="E336" t="s">
-        <v>979</v>
+        <v>972</v>
       </c>
     </row>
     <row r="337" spans="1:3" hidden="1" x14ac:dyDescent="0.75">
@@ -9253,7 +9374,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="424" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="424" spans="1:5" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A424" s="6" t="s">
         <v>832</v>
       </c>
@@ -9267,7 +9388,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="425" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A425" s="4" t="s">
         <v>832</v>
       </c>
@@ -9281,7 +9402,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="426" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A426" s="4" t="s">
         <v>832</v>
       </c>
@@ -9295,7 +9416,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="427" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A427" s="4" t="s">
         <v>832</v>
       </c>
@@ -9309,10 +9430,10 @@
         <v>910</v>
       </c>
       <c r="E427" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.75">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A428" s="4" t="s">
         <v>832</v>
       </c>
@@ -9326,7 +9447,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="429" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A429" s="4" t="s">
         <v>832</v>
       </c>
@@ -9340,7 +9461,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="430" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="430" spans="1:5" ht="77.25" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A430" s="4" t="s">
         <v>832</v>
       </c>
@@ -9354,7 +9475,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="431" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A431" s="4" t="s">
         <v>832</v>
       </c>
@@ -9368,7 +9489,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="432" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A432" s="4" t="s">
         <v>832</v>
       </c>
@@ -9382,7 +9503,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="433" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A433" s="4" t="s">
         <v>832</v>
       </c>
@@ -9396,10 +9517,10 @@
         <v>911</v>
       </c>
       <c r="E433" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.75">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A434" s="4" t="s">
         <v>832</v>
       </c>
@@ -9413,10 +9534,10 @@
         <v>911</v>
       </c>
       <c r="E434" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.75">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="435" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A435" s="4" t="s">
         <v>832</v>
       </c>
@@ -9430,7 +9551,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="436" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="436" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A436" s="4" t="s">
         <v>832</v>
       </c>
@@ -9444,7 +9565,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="437" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A437" s="4" t="s">
         <v>832</v>
       </c>
@@ -9458,7 +9579,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="438" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="438" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A438" s="4" t="s">
         <v>832</v>
       </c>
@@ -9472,7 +9593,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="439" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="439" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A439" s="4" t="s">
         <v>832</v>
       </c>
@@ -9486,7 +9607,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="440" spans="1:5" ht="60.45" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="440" spans="1:5" ht="60.45" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A440" s="4" t="s">
         <v>832</v>
       </c>
@@ -9500,7 +9621,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="441" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A441" s="4" t="s">
         <v>832</v>
       </c>
@@ -9517,7 +9638,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="442" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="442" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A442" s="4" t="s">
         <v>832</v>
       </c>
@@ -9531,7 +9652,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="443" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A443" s="4" t="s">
         <v>832</v>
       </c>
@@ -9545,7 +9666,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="444" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A444" s="4" t="s">
         <v>832</v>
       </c>
@@ -9559,7 +9680,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="445" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A445" s="4" t="s">
         <v>832</v>
       </c>
@@ -9573,7 +9694,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="446" spans="1:5" s="9" customFormat="1" ht="59" x14ac:dyDescent="0.75">
+    <row r="446" spans="1:5" s="9" customFormat="1" ht="59" hidden="1" x14ac:dyDescent="0.75">
       <c r="A446" s="6" t="s">
         <v>832</v>
       </c>
@@ -9587,7 +9708,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="447" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A447" s="4" t="s">
         <v>832</v>
       </c>
@@ -9601,7 +9722,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="448" spans="1:5" ht="59" x14ac:dyDescent="0.75">
+    <row r="448" spans="1:5" ht="59" hidden="1" x14ac:dyDescent="0.75">
       <c r="A448" s="4" t="s">
         <v>832</v>
       </c>
@@ -9615,7 +9736,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="449" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="449" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A449" s="4" t="s">
         <v>832</v>
       </c>
@@ -9629,7 +9750,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="450" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="450" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A450" s="4" t="s">
         <v>832</v>
       </c>
@@ -9643,7 +9764,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="451" spans="1:5" ht="45.45" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="451" spans="1:5" ht="45.45" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A451" s="4" t="s">
         <v>832</v>
       </c>
@@ -9657,7 +9778,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="452" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="452" spans="1:5" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A452" s="6" t="s">
         <v>889</v>
       </c>
@@ -9671,7 +9792,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="453" spans="1:5" s="9" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="453" spans="1:5" s="9" customFormat="1" ht="30.45" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A453" s="6" t="s">
         <v>889</v>
       </c>
@@ -9685,7 +9806,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="454" spans="1:5" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="454" spans="1:5" s="9" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A454" s="6" t="s">
         <v>889</v>
       </c>
@@ -9699,7 +9820,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="455" spans="1:5" s="9" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="455" spans="1:5" s="9" customFormat="1" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A455" s="6" t="s">
         <v>889</v>
       </c>
@@ -9713,7 +9834,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="456" spans="1:5" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="456" spans="1:5" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A456" s="6" t="s">
         <v>889</v>
       </c>
@@ -9727,7 +9848,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="457" spans="1:5" s="9" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="457" spans="1:5" s="9" customFormat="1" ht="30.45" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A457" s="6" t="s">
         <v>889</v>
       </c>
@@ -9741,7 +9862,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="458" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="458" spans="1:5" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A458" s="6" t="s">
         <v>889</v>
       </c>
@@ -9755,7 +9876,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="459" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="459" spans="1:5" ht="28.95" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A459" s="6" t="s">
         <v>889</v>
       </c>
@@ -9769,7 +9890,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="460" spans="1:5" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="460" spans="1:5" ht="32.700000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A460" s="6" t="s">
         <v>889</v>
       </c>
@@ -9783,7 +9904,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="461" spans="1:5" ht="23.7" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="461" spans="1:5" ht="23.7" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A461" s="6" t="s">
         <v>889</v>
       </c>
@@ -9797,7 +9918,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="462" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="462" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A462" s="6" t="s">
         <v>889</v>
       </c>
@@ -9811,7 +9932,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="463" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="463" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A463" s="6" t="s">
         <v>889</v>
       </c>
@@ -9825,10 +9946,10 @@
         <v>911</v>
       </c>
       <c r="E463" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="464" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A464" s="6" t="s">
         <v>832</v>
       </c>
@@ -9842,7 +9963,7 @@
         <v>911</v>
       </c>
       <c r="E464" t="s">
-        <v>977</v>
+        <v>970</v>
       </c>
     </row>
     <row r="465" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
@@ -9856,7 +9977,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="466" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="466" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A466" s="4" t="s">
         <v>7</v>
       </c>
@@ -9870,11 +9991,16 @@
         <v>911</v>
       </c>
       <c r="E466" t="s">
-        <v>997</v>
+        <v>989</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E466" xr:uid="{00252C19-57C4-4095-B3AB-85A45AD6EFCF}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="PolLimit1Building"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="3">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10093,19 +10219,22 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B2:F53"/>
+  <dimension ref="B2:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="2" max="2" width="21.86328125" customWidth="1"/>
-    <col min="3" max="3" width="15.6796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
     <col min="4" max="4" width="35.54296875" customWidth="1"/>
     <col min="5" max="5" width="59.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26" x14ac:dyDescent="1.2">
@@ -10123,7 +10252,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B6" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.75">
@@ -10138,7 +10267,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B9" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.75">
@@ -10243,7 +10372,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.75">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.75">
       <c r="B17" t="s">
         <v>933</v>
       </c>
@@ -10260,7 +10389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.75">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.75">
       <c r="B18" t="s">
         <v>933</v>
       </c>
@@ -10277,7 +10406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.75">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.75">
       <c r="B19" t="s">
         <v>934</v>
       </c>
@@ -10294,232 +10423,380 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="18.5" x14ac:dyDescent="0.9">
+    <row r="21" spans="2:9" ht="18.5" x14ac:dyDescent="0.9">
       <c r="B21" s="21" t="s">
         <v>956</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B23" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B24" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B26" s="22" t="s">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B22" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B24" s="26" t="s">
+        <v>871</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>997</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>845</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>849</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>847</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>853</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>851</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B25" s="26" t="s">
+        <v>994</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>998</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B26" s="26" t="s">
+        <v>992</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>999</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B27" s="26" t="s">
+        <v>993</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B28" s="26" t="s">
+        <v>995</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B29" s="26" t="s">
+        <v>996</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H29" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B31" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B33" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B34" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B36" s="22" t="s">
         <v>958</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C36" s="22" t="s">
         <v>939</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D36" s="22" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B27">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B37">
         <v>1</v>
       </c>
-      <c r="C27">
+      <c r="C37">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D37" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B28">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B38">
         <v>2</v>
       </c>
-      <c r="C28">
+      <c r="C38">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D38" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B29">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B39">
         <v>3</v>
       </c>
-      <c r="C29">
+      <c r="C39">
         <v>1</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D39" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B30">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B40">
         <v>4</v>
       </c>
-      <c r="C30">
+      <c r="C40">
         <v>1</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D40" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B31">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B41">
         <v>5</v>
       </c>
-      <c r="C31">
+      <c r="C41">
         <v>2</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D41" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B32">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B42">
         <v>6</v>
       </c>
-      <c r="C32">
+      <c r="C42">
         <v>2</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D42" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B33">
-        <v>7</v>
-      </c>
-      <c r="C33">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="C43">
         <v>2</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D43" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B34">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B44">
         <v>8</v>
       </c>
-      <c r="C34">
+      <c r="C44">
         <v>2</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D44" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B35">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B45">
         <v>9</v>
       </c>
-      <c r="C35">
+      <c r="C45">
         <v>3</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D45" t="s">
         <v>947</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B37" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B38" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B39" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B40" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B41" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B42" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B44" s="1" t="s">
-        <v>929</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>935</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B45" t="s">
-        <v>963</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B46" t="s">
-        <v>962</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B47" t="s">
-        <v>966</v>
-      </c>
-      <c r="C47">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B48" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B49" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B50" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B51" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B54" s="22" t="s">
+        <v>929</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>935</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B55" t="s">
+        <v>961</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B56" t="s">
+        <v>960</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B57" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C57">
         <v>3</v>
       </c>
-      <c r="D47" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="18.5" x14ac:dyDescent="0.9">
-      <c r="B50" s="21" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.75">
-      <c r="B51" t="s">
-        <v>991</v>
-      </c>
-      <c r="C51" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.75">
-      <c r="B52" t="s">
-        <v>986</v>
-      </c>
-      <c r="C52" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.75">
-      <c r="B53" t="s">
-        <v>990</v>
-      </c>
-      <c r="C53" t="s">
-        <v>989</v>
+      <c r="D57" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" ht="18.5" x14ac:dyDescent="0.9">
+      <c r="B60" s="21" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B61" t="s">
+        <v>983</v>
+      </c>
+      <c r="C61" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B62" t="s">
+        <v>978</v>
+      </c>
+      <c r="C62" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B63" t="s">
+        <v>982</v>
+      </c>
+      <c r="C63" t="s">
+        <v>981</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more information about supported reinsurance fields for different contract types (#1102)
</commit_message>
<xml_diff>
--- a/docs/OED_financial_terms_supported.xlsx
+++ b/docs/OED_financial_terms_supported.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_backallocation2\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\joh\dev\OasisLMF_update-fm-docs\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BD5F59-DB1F-499E-B7EB-3A613DE845D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5C6EB2-42D1-49A2-8DE3-189226CB6E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25507" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
+    <workbookView xWindow="28000" yWindow="2400" windowWidth="19200" windowHeight="9900" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="1000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="1014">
   <si>
     <t>File Name</t>
   </si>
@@ -2975,15 +2975,9 @@
     <t>Cycle</t>
   </si>
   <si>
-    <t xml:space="preserve">The terms are applied in the order of processing cycle. The net loss is output from each processing cycle and feeds into the next processing cycle. </t>
-  </si>
-  <si>
     <t>The calculated loss is passed from one level to the next, and the output from the final level is the gross loss.</t>
   </si>
   <si>
-    <t>Within each cycle there are three fixed levels of calculation.</t>
-  </si>
-  <si>
     <t>Risk level</t>
   </si>
   <si>
@@ -2996,27 +2990,12 @@
     <t>OccAttachment, OccLimit, PlacedPercent</t>
   </si>
   <si>
-    <t>Layer level</t>
-  </si>
-  <si>
     <t>The final step is to difference the input and the output, and pass through the net loss to the next processing cycle.</t>
   </si>
   <si>
-    <t>The first level groups losses by location and by policy. The calculation filters losses that are within the scope of each reinsurance layer and passes them through to the next level. All other losses are set to zero.</t>
-  </si>
-  <si>
     <t>All supported direct insurance terms are associated with a fixed 'FM level'. The level specifies how losses should be grouped together for processing.</t>
   </si>
   <si>
-    <t>Each Reinsurance layer (identified by ReinsNumber) is allocated to a processing cycle depending on the InuringPriority and RiskLevel. The number of cycles will vary depending on the data in the ri_info and ri_scope file</t>
-  </si>
-  <si>
-    <t>The second level groups loss to the Risk Level (either location, or policy, or account) and applies the CededPercent and then any risk terms to the losses.</t>
-  </si>
-  <si>
-    <t>The third level groups losses to the Layer level (which means summing losses across all risks in scope of the reinsurance layer) and applies the occurrence terms and finally the PlacedPercent which results in the Reinsurance layer loss</t>
-  </si>
-  <si>
     <t>Order of Operation</t>
   </si>
   <si>
@@ -3050,9 +3029,6 @@
     <t>Is the field supported by the OasisLMF financial module (Yes/No/(blank))</t>
   </si>
   <si>
-    <t>The order of terms appled within each level is determined by a specific calcrule that is invoked by the calculation.</t>
-  </si>
-  <si>
     <t>References</t>
   </si>
   <si>
@@ -3096,6 +3072,132 @@
   </si>
   <si>
     <t>v1.26</t>
+  </si>
+  <si>
+    <t>QS</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>FAC</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>CXL</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Facultative</t>
+  </si>
+  <si>
+    <t>Quota Share</t>
+  </si>
+  <si>
+    <t>Surplus Share</t>
+  </si>
+  <si>
+    <t>Catastrophe Excess of Loss</t>
+  </si>
+  <si>
+    <t>Per Risk Excess of Loss</t>
+  </si>
+  <si>
+    <t>Each Reinsurance contract (identified by ReinsNumber) is allocated to a processing cycle depending on the InuringPriority and RiskLevel. The number of cycles will vary depending on the data in the ri_info and ri_scope file</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x*</t>
+  </si>
+  <si>
+    <t>*Only for Surplus Share is CededPercent specified per risk and taken from the reinsurance scope file. All other reinsurance types use the CededPercent in the reinsurance info file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The contracts are allocated to a processing cycle based on InuringPriority and RiskLevel and processed in cycle order. The net loss is output from each processing cycle and feeds into the next processing cycle. </t>
+  </si>
+  <si>
+    <t>Contract level</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Location Policy Level: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The first level sums losses by location and by policy. The calculation filters losses that are within the scope of each reinsurance layer and passes them through to the next level. All other losses are set to zero because they are outside the scope of the contract.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Risk Level:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The second level sums loss to the Risk Level (either location, or policy, or account) and applies the CededPercent and then any risk terms to the losses.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Contract Level: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The third level groups losses to the contract level (which means summing losses across all risks in scope of the reinsurance layer) and applies the occurrence terms and finally the PlacedPercent which results in the Reinsurance contract loss</t>
+    </r>
+  </si>
+  <si>
+    <t>Within each cycle there are three fixed levels of calculation. Each level involves summing losses and then applying a financial terms calculation.</t>
+  </si>
+  <si>
+    <t>The following types of reinsurance are supported and use the fields in reinsurance info and reinsurance scope files indicated in the matrix</t>
   </si>
 </sst>
 </file>
@@ -3171,7 +3273,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -3179,12 +3281,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3245,6 +3362,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3641,7 +3762,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B4" t="s">
-        <v>978</v>
+        <v>971</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.75">
@@ -3649,13 +3770,13 @@
         <v>925</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>998</v>
+        <v>990</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>926</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>999</v>
+        <v>991</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.75">
@@ -3668,7 +3789,7 @@
         <v>922</v>
       </c>
       <c r="F9" t="s">
-        <v>982</v>
+        <v>975</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.75">
@@ -3692,7 +3813,7 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>981</v>
+        <v>974</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.75">
@@ -3700,7 +3821,7 @@
         <v>908</v>
       </c>
       <c r="G13" t="s">
-        <v>983</v>
+        <v>976</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.75">
@@ -3713,10 +3834,10 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.75">
       <c r="B16" s="25" t="s">
-        <v>973</v>
+        <v>966</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>974</v>
+        <v>967</v>
       </c>
     </row>
   </sheetData>
@@ -3736,8 +3857,8 @@
   <dimension ref="A1:E466"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3766,7 +3887,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -3802,7 +3923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -3827,7 +3948,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -3853,7 +3974,7 @@
       </c>
       <c r="D8" s="16"/>
     </row>
-    <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -3878,7 +3999,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -3961,7 +4082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -3975,10 +4096,10 @@
         <v>910</v>
       </c>
       <c r="E18" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -3992,7 +4113,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
@@ -4006,7 +4127,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -4020,7 +4141,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
@@ -4034,7 +4155,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
@@ -4048,7 +4169,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -4062,7 +4183,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A25" s="4" t="s">
         <v>7</v>
       </c>
@@ -4076,7 +4197,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -4090,7 +4211,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
@@ -4104,7 +4225,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
@@ -4118,7 +4239,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -4132,7 +4253,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A30" s="4" t="s">
         <v>7</v>
       </c>
@@ -4146,7 +4267,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -4160,7 +4281,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A32" s="4" t="s">
         <v>7</v>
       </c>
@@ -4174,7 +4295,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A33" s="4" t="s">
         <v>7</v>
       </c>
@@ -4188,7 +4309,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
@@ -4202,7 +4323,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A35" s="4" t="s">
         <v>7</v>
       </c>
@@ -4216,7 +4337,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A36" s="4" t="s">
         <v>7</v>
       </c>
@@ -4230,7 +4351,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
@@ -4244,7 +4365,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A38" s="4" t="s">
         <v>7</v>
       </c>
@@ -4258,7 +4379,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
@@ -4272,7 +4393,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A40" s="4" t="s">
         <v>7</v>
       </c>
@@ -4286,7 +4407,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A41" s="4" t="s">
         <v>7</v>
       </c>
@@ -4300,7 +4421,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
@@ -4314,7 +4435,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A43" s="4" t="s">
         <v>7</v>
       </c>
@@ -4328,7 +4449,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -4342,7 +4463,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
@@ -4356,7 +4477,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -4370,7 +4491,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -4384,7 +4505,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A48" s="4" t="s">
         <v>7</v>
       </c>
@@ -4398,7 +4519,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
@@ -4412,7 +4533,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A50" s="4" t="s">
         <v>7</v>
       </c>
@@ -4426,7 +4547,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A51" s="4" t="s">
         <v>7</v>
       </c>
@@ -4440,7 +4561,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A52" s="4" t="s">
         <v>7</v>
       </c>
@@ -4454,7 +4575,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A53" s="4" t="s">
         <v>7</v>
       </c>
@@ -4468,7 +4589,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -4482,7 +4603,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A55" s="4" t="s">
         <v>7</v>
       </c>
@@ -4496,7 +4617,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A56" s="4" t="s">
         <v>7</v>
       </c>
@@ -4510,7 +4631,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A57" s="4" t="s">
         <v>7</v>
       </c>
@@ -4524,7 +4645,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A58" s="4" t="s">
         <v>7</v>
       </c>
@@ -4538,7 +4659,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A59" s="4" t="s">
         <v>7</v>
       </c>
@@ -4552,7 +4673,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A60" s="4" t="s">
         <v>7</v>
       </c>
@@ -4566,7 +4687,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A61" s="4" t="s">
         <v>7</v>
       </c>
@@ -4580,7 +4701,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
@@ -4594,7 +4715,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A63" s="4" t="s">
         <v>7</v>
       </c>
@@ -4608,7 +4729,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A64" s="4" t="s">
         <v>7</v>
       </c>
@@ -4622,7 +4743,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A65" s="4" t="s">
         <v>7</v>
       </c>
@@ -4636,7 +4757,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A66" s="4" t="s">
         <v>7</v>
       </c>
@@ -4650,7 +4771,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A67" s="4" t="s">
         <v>7</v>
       </c>
@@ -4664,7 +4785,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A68" s="4" t="s">
         <v>7</v>
       </c>
@@ -4678,7 +4799,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A69" s="4" t="s">
         <v>7</v>
       </c>
@@ -4692,7 +4813,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A70" s="4" t="s">
         <v>7</v>
       </c>
@@ -4750,7 +4871,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:5" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A75" s="6" t="s">
         <v>7</v>
       </c>
@@ -4764,7 +4885,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A76" s="4" t="s">
         <v>7</v>
       </c>
@@ -4781,7 +4902,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A77" s="4" t="s">
         <v>7</v>
       </c>
@@ -4795,7 +4916,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
@@ -4809,7 +4930,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A79" s="4" t="s">
         <v>7</v>
       </c>
@@ -4823,7 +4944,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A80" s="4" t="s">
         <v>7</v>
       </c>
@@ -4837,7 +4958,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A81" s="4" t="s">
         <v>7</v>
       </c>
@@ -4854,7 +4975,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A82" s="4" t="s">
         <v>7</v>
       </c>
@@ -4871,7 +4992,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A83" s="4" t="s">
         <v>7</v>
       </c>
@@ -4888,7 +5009,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A84" s="4" t="s">
         <v>7</v>
       </c>
@@ -4902,7 +5023,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:5" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
       <c r="A85" s="4" t="s">
         <v>7</v>
       </c>
@@ -4916,7 +5037,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
@@ -4930,10 +5051,10 @@
         <v>910</v>
       </c>
       <c r="E86" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.75">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A87" s="4" t="s">
         <v>7</v>
       </c>
@@ -4947,7 +5068,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A88" s="4" t="s">
         <v>7</v>
       </c>
@@ -4961,7 +5082,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A89" s="4" t="s">
         <v>7</v>
       </c>
@@ -4975,7 +5096,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A90" s="4" t="s">
         <v>7</v>
       </c>
@@ -4989,7 +5110,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A91" s="4" t="s">
         <v>7</v>
       </c>
@@ -5003,7 +5124,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A92" s="4" t="s">
         <v>7</v>
       </c>
@@ -5017,7 +5138,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A93" s="4" t="s">
         <v>7</v>
       </c>
@@ -5031,7 +5152,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
@@ -5045,7 +5166,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A95" s="4" t="s">
         <v>7</v>
       </c>
@@ -5059,7 +5180,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A96" s="4" t="s">
         <v>7</v>
       </c>
@@ -5073,7 +5194,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A97" s="4" t="s">
         <v>7</v>
       </c>
@@ -5087,7 +5208,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A98" s="4" t="s">
         <v>7</v>
       </c>
@@ -5101,7 +5222,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A99" s="4" t="s">
         <v>7</v>
       </c>
@@ -5115,7 +5236,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A100" s="4" t="s">
         <v>7</v>
       </c>
@@ -5129,7 +5250,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A101" s="4" t="s">
         <v>7</v>
       </c>
@@ -5143,7 +5264,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
@@ -5157,7 +5278,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A103" s="4" t="s">
         <v>7</v>
       </c>
@@ -5171,7 +5292,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A104" s="4" t="s">
         <v>7</v>
       </c>
@@ -5185,7 +5306,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A105" s="4" t="s">
         <v>7</v>
       </c>
@@ -5199,7 +5320,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A106" s="4" t="s">
         <v>7</v>
       </c>
@@ -5213,7 +5334,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A107" s="4" t="s">
         <v>7</v>
       </c>
@@ -5227,7 +5348,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A108" s="4" t="s">
         <v>7</v>
       </c>
@@ -5241,7 +5362,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A109" s="4" t="s">
         <v>7</v>
       </c>
@@ -5255,7 +5376,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
@@ -5269,7 +5390,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A111" s="4" t="s">
         <v>7</v>
       </c>
@@ -5283,7 +5404,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A112" s="4" t="s">
         <v>7</v>
       </c>
@@ -5297,7 +5418,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A113" s="4" t="s">
         <v>7</v>
       </c>
@@ -5311,7 +5432,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A114" s="4" t="s">
         <v>7</v>
       </c>
@@ -5325,7 +5446,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A115" s="4" t="s">
         <v>7</v>
       </c>
@@ -5339,7 +5460,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A116" s="4" t="s">
         <v>7</v>
       </c>
@@ -5353,7 +5474,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A117" s="4" t="s">
         <v>7</v>
       </c>
@@ -5367,7 +5488,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A118" s="4" t="s">
         <v>7</v>
       </c>
@@ -5395,7 +5516,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A120" s="4" t="s">
         <v>7</v>
       </c>
@@ -5409,7 +5530,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A121" s="4" t="s">
         <v>7</v>
       </c>
@@ -5423,7 +5544,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A122" s="4" t="s">
         <v>7</v>
       </c>
@@ -5437,7 +5558,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A123" s="4" t="s">
         <v>7</v>
       </c>
@@ -5451,7 +5572,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A124" s="4" t="s">
         <v>7</v>
       </c>
@@ -5465,7 +5586,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A125" s="4" t="s">
         <v>7</v>
       </c>
@@ -5479,7 +5600,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A126" s="4" t="s">
         <v>7</v>
       </c>
@@ -5493,7 +5614,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A127" s="4" t="s">
         <v>7</v>
       </c>
@@ -5507,7 +5628,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A128" s="4" t="s">
         <v>7</v>
       </c>
@@ -5521,7 +5642,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A129" s="4" t="s">
         <v>7</v>
       </c>
@@ -5535,7 +5656,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A130" s="4" t="s">
         <v>7</v>
       </c>
@@ -5549,7 +5670,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A131" s="4" t="s">
         <v>7</v>
       </c>
@@ -5563,7 +5684,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A132" s="4" t="s">
         <v>7</v>
       </c>
@@ -5577,7 +5698,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A133" s="4" t="s">
         <v>7</v>
       </c>
@@ -5591,7 +5712,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A134" s="4" t="s">
         <v>7</v>
       </c>
@@ -5605,7 +5726,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A135" s="4" t="s">
         <v>7</v>
       </c>
@@ -5619,7 +5740,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A136" s="4" t="s">
         <v>7</v>
       </c>
@@ -5633,7 +5754,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A137" s="4" t="s">
         <v>7</v>
       </c>
@@ -5647,7 +5768,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A138" s="4" t="s">
         <v>7</v>
       </c>
@@ -5661,7 +5782,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A139" s="4" t="s">
         <v>7</v>
       </c>
@@ -5675,7 +5796,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A140" s="4" t="s">
         <v>7</v>
       </c>
@@ -5689,7 +5810,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A141" s="4" t="s">
         <v>7</v>
       </c>
@@ -5703,7 +5824,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A142" s="4" t="s">
         <v>7</v>
       </c>
@@ -5717,7 +5838,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A143" s="4" t="s">
         <v>7</v>
       </c>
@@ -5731,7 +5852,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:4" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
       <c r="A144" s="4" t="s">
         <v>7</v>
       </c>
@@ -5745,7 +5866,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A145" s="4" t="s">
         <v>7</v>
       </c>
@@ -5759,7 +5880,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A146" s="4" t="s">
         <v>7</v>
       </c>
@@ -5773,7 +5894,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A147" s="4" t="s">
         <v>7</v>
       </c>
@@ -5787,7 +5908,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A148" s="4" t="s">
         <v>7</v>
       </c>
@@ -5801,7 +5922,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A149" s="4" t="s">
         <v>7</v>
       </c>
@@ -5815,7 +5936,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:4" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
       <c r="A150" s="4" t="s">
         <v>7</v>
       </c>
@@ -5829,7 +5950,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A151" s="4" t="s">
         <v>7</v>
       </c>
@@ -5843,7 +5964,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A152" s="4" t="s">
         <v>7</v>
       </c>
@@ -5857,7 +5978,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A153" s="4" t="s">
         <v>7</v>
       </c>
@@ -5871,7 +5992,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:4" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A154" s="4" t="s">
         <v>7</v>
       </c>
@@ -5885,7 +6006,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="42.45" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:4" ht="42.45" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A155" s="4" t="s">
         <v>7</v>
       </c>
@@ -5899,7 +6020,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="59.7" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:4" ht="59.7" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A156" s="4" t="s">
         <v>7</v>
       </c>
@@ -5913,7 +6034,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A157" s="4" t="s">
         <v>7</v>
       </c>
@@ -5927,7 +6048,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:4" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
       <c r="A158" s="4" t="s">
         <v>7</v>
       </c>
@@ -5941,7 +6062,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A159" s="4" t="s">
         <v>7</v>
       </c>
@@ -5955,7 +6076,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="59" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:4" ht="59" hidden="1" x14ac:dyDescent="0.75">
       <c r="A160" s="4" t="s">
         <v>7</v>
       </c>
@@ -5969,7 +6090,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A161" s="4" t="s">
         <v>7</v>
       </c>
@@ -5983,7 +6104,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:5" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
       <c r="A162" s="4" t="s">
         <v>7</v>
       </c>
@@ -5997,7 +6118,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A163" s="4" t="s">
         <v>7</v>
       </c>
@@ -6077,21 +6198,21 @@
         <v>337</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A170" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>993</v>
+        <v>985</v>
       </c>
       <c r="D170" s="16" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="171" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A171" s="4" t="s">
         <v>7</v>
       </c>
@@ -6099,13 +6220,13 @@
         <v>338</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>994</v>
+        <v>986</v>
       </c>
       <c r="D171" s="16" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A172" s="4" t="s">
         <v>7</v>
       </c>
@@ -6113,13 +6234,13 @@
         <v>339</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>995</v>
+        <v>987</v>
       </c>
       <c r="D172" s="16" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="173" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A173" s="4" t="s">
         <v>7</v>
       </c>
@@ -6133,7 +6254,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A174" s="4" t="s">
         <v>7</v>
       </c>
@@ -6147,10 +6268,10 @@
         <v>910</v>
       </c>
       <c r="E174" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.75">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A175" s="4" t="s">
         <v>7</v>
       </c>
@@ -6164,7 +6285,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A176" s="4" t="s">
         <v>7</v>
       </c>
@@ -6178,7 +6299,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A177" s="4" t="s">
         <v>7</v>
       </c>
@@ -6192,7 +6313,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A178" s="4" t="s">
         <v>7</v>
       </c>
@@ -6206,7 +6327,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A179" s="4" t="s">
         <v>7</v>
       </c>
@@ -6220,7 +6341,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A180" s="4" t="s">
         <v>7</v>
       </c>
@@ -6234,7 +6355,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A181" s="4" t="s">
         <v>7</v>
       </c>
@@ -6248,7 +6369,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A182" s="4" t="s">
         <v>7</v>
       </c>
@@ -6262,7 +6383,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A183" s="4" t="s">
         <v>7</v>
       </c>
@@ -6276,7 +6397,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A184" s="4" t="s">
         <v>7</v>
       </c>
@@ -6290,7 +6411,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A185" s="4" t="s">
         <v>7</v>
       </c>
@@ -6304,7 +6425,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A186" s="4" t="s">
         <v>7</v>
       </c>
@@ -6318,7 +6439,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A187" s="4" t="s">
         <v>7</v>
       </c>
@@ -6332,7 +6453,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A188" s="4" t="s">
         <v>7</v>
       </c>
@@ -6346,7 +6467,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A189" s="4" t="s">
         <v>7</v>
       </c>
@@ -6360,7 +6481,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A190" s="4" t="s">
         <v>7</v>
       </c>
@@ -6374,7 +6495,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A191" s="4" t="s">
         <v>7</v>
       </c>
@@ -6388,7 +6509,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A192" s="4" t="s">
         <v>7</v>
       </c>
@@ -6402,7 +6523,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A193" s="4" t="s">
         <v>7</v>
       </c>
@@ -6416,7 +6537,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A194" s="4" t="s">
         <v>7</v>
       </c>
@@ -6430,7 +6551,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A195" s="4" t="s">
         <v>7</v>
       </c>
@@ -6444,7 +6565,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A196" s="4" t="s">
         <v>7</v>
       </c>
@@ -6458,7 +6579,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A197" s="4" t="s">
         <v>7</v>
       </c>
@@ -6472,7 +6593,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A198" s="4" t="s">
         <v>7</v>
       </c>
@@ -6486,7 +6607,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A199" s="4" t="s">
         <v>7</v>
       </c>
@@ -6500,7 +6621,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A200" s="4" t="s">
         <v>7</v>
       </c>
@@ -6514,7 +6635,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A201" s="4" t="s">
         <v>7</v>
       </c>
@@ -6528,7 +6649,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A202" s="4" t="s">
         <v>7</v>
       </c>
@@ -6542,10 +6663,10 @@
         <v>911</v>
       </c>
       <c r="E202" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.75">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A203" s="4" t="s">
         <v>7</v>
       </c>
@@ -6559,10 +6680,10 @@
         <v>911</v>
       </c>
       <c r="E203" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.75">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A204" s="4" t="s">
         <v>7</v>
       </c>
@@ -6576,10 +6697,10 @@
         <v>911</v>
       </c>
       <c r="E204" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.75">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A205" s="4" t="s">
         <v>7</v>
       </c>
@@ -6593,7 +6714,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A206" s="4" t="s">
         <v>7</v>
       </c>
@@ -6607,7 +6728,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A207" s="4" t="s">
         <v>7</v>
       </c>
@@ -6621,7 +6742,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A208" s="4" t="s">
         <v>7</v>
       </c>
@@ -6635,7 +6756,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A209" s="4" t="s">
         <v>7</v>
       </c>
@@ -6649,7 +6770,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A210" s="4" t="s">
         <v>7</v>
       </c>
@@ -6663,7 +6784,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A211" s="4" t="s">
         <v>7</v>
       </c>
@@ -6677,7 +6798,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A212" s="4" t="s">
         <v>7</v>
       </c>
@@ -6691,7 +6812,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A213" s="4" t="s">
         <v>7</v>
       </c>
@@ -6705,7 +6826,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A214" s="4" t="s">
         <v>7</v>
       </c>
@@ -6719,7 +6840,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A215" s="4" t="s">
         <v>7</v>
       </c>
@@ -6733,7 +6854,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A216" s="4" t="s">
         <v>7</v>
       </c>
@@ -6747,7 +6868,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A217" s="4" t="s">
         <v>7</v>
       </c>
@@ -6761,7 +6882,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A218" s="4" t="s">
         <v>7</v>
       </c>
@@ -6775,7 +6896,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A219" s="4" t="s">
         <v>7</v>
       </c>
@@ -6789,7 +6910,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A220" s="4" t="s">
         <v>7</v>
       </c>
@@ -6803,7 +6924,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A221" s="4" t="s">
         <v>7</v>
       </c>
@@ -6817,7 +6938,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A222" s="4" t="s">
         <v>7</v>
       </c>
@@ -6831,7 +6952,7 @@
         <v>911</v>
       </c>
       <c r="E222" t="s">
-        <v>975</v>
+        <v>968</v>
       </c>
     </row>
     <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
@@ -7374,7 +7495,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="272" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A272" s="4" t="s">
         <v>440</v>
       </c>
@@ -7388,10 +7509,10 @@
         <v>911</v>
       </c>
       <c r="E272" t="s">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.75">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A273" s="4" t="s">
         <v>440</v>
       </c>
@@ -7405,7 +7526,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="274" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="274" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A274" s="4" t="s">
         <v>440</v>
       </c>
@@ -7422,7 +7543,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A275" s="4" t="s">
         <v>440</v>
       </c>
@@ -7436,7 +7557,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A276" s="4" t="s">
         <v>440</v>
       </c>
@@ -7453,7 +7574,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="277" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="277" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A277" s="4" t="s">
         <v>440</v>
       </c>
@@ -7467,7 +7588,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A278" s="4" t="s">
         <v>440</v>
       </c>
@@ -7484,7 +7605,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A279" s="6" t="s">
         <v>440</v>
       </c>
@@ -7498,7 +7619,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A280" s="6" t="s">
         <v>440</v>
       </c>
@@ -7512,7 +7633,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A281" s="6" t="s">
         <v>440</v>
       </c>
@@ -7526,7 +7647,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A282" s="6" t="s">
         <v>440</v>
       </c>
@@ -7540,7 +7661,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A283" s="6" t="s">
         <v>440</v>
       </c>
@@ -7554,7 +7675,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="284" spans="1:5" ht="43.95" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="284" spans="1:5" ht="43.95" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A284" s="6" t="s">
         <v>440</v>
       </c>
@@ -7568,7 +7689,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="285" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="285" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A285" s="6" t="s">
         <v>440</v>
       </c>
@@ -7593,7 +7714,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A287" s="4" t="s">
         <v>440</v>
       </c>
@@ -7607,7 +7728,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A288" s="4" t="s">
         <v>440</v>
       </c>
@@ -7621,7 +7742,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="289" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A289" s="4" t="s">
         <v>440</v>
       </c>
@@ -7635,7 +7756,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="290" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A290" s="4" t="s">
         <v>440</v>
       </c>
@@ -7649,7 +7770,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="291" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A291" s="4" t="s">
         <v>440</v>
       </c>
@@ -7663,7 +7784,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="292" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A292" s="4" t="s">
         <v>440</v>
       </c>
@@ -7677,7 +7798,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="293" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A293" s="4" t="s">
         <v>440</v>
       </c>
@@ -7691,7 +7812,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="294" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A294" s="4" t="s">
         <v>440</v>
       </c>
@@ -7705,7 +7826,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="295" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A295" s="4" t="s">
         <v>440</v>
       </c>
@@ -7719,7 +7840,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="296" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A296" s="4" t="s">
         <v>440</v>
       </c>
@@ -7733,7 +7854,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="297" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A297" s="4" t="s">
         <v>440</v>
       </c>
@@ -7747,7 +7868,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="298" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A298" s="4" t="s">
         <v>440</v>
       </c>
@@ -7761,7 +7882,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="299" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A299" s="4" t="s">
         <v>440</v>
       </c>
@@ -7775,7 +7896,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="300" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A300" s="4" t="s">
         <v>440</v>
       </c>
@@ -7789,7 +7910,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="301" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A301" s="4" t="s">
         <v>440</v>
       </c>
@@ -7803,7 +7924,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="302" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A302" s="4" t="s">
         <v>440</v>
       </c>
@@ -7817,7 +7938,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="303" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A303" s="4" t="s">
         <v>440</v>
       </c>
@@ -7831,7 +7952,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="304" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A304" s="4" t="s">
         <v>440</v>
       </c>
@@ -7845,7 +7966,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="305" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A305" s="4" t="s">
         <v>440</v>
       </c>
@@ -7859,7 +7980,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="306" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A306" s="4" t="s">
         <v>440</v>
       </c>
@@ -7873,7 +7994,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="307" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A307" s="4" t="s">
         <v>440</v>
       </c>
@@ -7887,7 +8008,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="308" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A308" s="4" t="s">
         <v>440</v>
       </c>
@@ -7901,7 +8022,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="309" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A309" s="4" t="s">
         <v>440</v>
       </c>
@@ -7915,7 +8036,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="310" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A310" s="4" t="s">
         <v>440</v>
       </c>
@@ -7929,7 +8050,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="311" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A311" s="4" t="s">
         <v>440</v>
       </c>
@@ -7943,7 +8064,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="312" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A312" s="4" t="s">
         <v>440</v>
       </c>
@@ -7957,7 +8078,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="313" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A313" s="4" t="s">
         <v>440</v>
       </c>
@@ -7971,7 +8092,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="314" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A314" s="4" t="s">
         <v>440</v>
       </c>
@@ -7985,7 +8106,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="315" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A315" s="4" t="s">
         <v>440</v>
       </c>
@@ -7999,7 +8120,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="316" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A316" s="4" t="s">
         <v>440</v>
       </c>
@@ -8013,7 +8134,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="317" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A317" s="4" t="s">
         <v>440</v>
       </c>
@@ -8027,7 +8148,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="318" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A318" s="4" t="s">
         <v>440</v>
       </c>
@@ -8041,7 +8162,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="319" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A319" s="4" t="s">
         <v>440</v>
       </c>
@@ -8055,7 +8176,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="320" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
       <c r="A320" s="4" t="s">
         <v>440</v>
       </c>
@@ -8069,7 +8190,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A321" s="4" t="s">
         <v>440</v>
       </c>
@@ -8083,7 +8204,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A322" s="4" t="s">
         <v>440</v>
       </c>
@@ -8097,7 +8218,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A323" s="4" t="s">
         <v>440</v>
       </c>
@@ -8111,7 +8232,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A324" s="4" t="s">
         <v>440</v>
       </c>
@@ -8125,7 +8246,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A325" s="4" t="s">
         <v>440</v>
       </c>
@@ -8139,7 +8260,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A326" s="4" t="s">
         <v>440</v>
       </c>
@@ -8153,7 +8274,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A327" s="4" t="s">
         <v>440</v>
       </c>
@@ -8167,7 +8288,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A328" s="4" t="s">
         <v>440</v>
       </c>
@@ -8181,7 +8302,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A329" s="4" t="s">
         <v>440</v>
       </c>
@@ -8195,7 +8316,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A330" s="4" t="s">
         <v>440</v>
       </c>
@@ -8209,7 +8330,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A331" s="4" t="s">
         <v>440</v>
       </c>
@@ -8223,7 +8344,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A332" s="4" t="s">
         <v>440</v>
       </c>
@@ -8237,7 +8358,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A333" s="4" t="s">
         <v>440</v>
       </c>
@@ -8251,7 +8372,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="334" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A334" s="4" t="s">
         <v>440</v>
       </c>
@@ -8265,7 +8386,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A335" s="4" t="s">
         <v>440</v>
       </c>
@@ -8279,7 +8400,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="336" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A336" s="6" t="s">
         <v>440</v>
       </c>
@@ -8293,7 +8414,7 @@
         <v>910</v>
       </c>
       <c r="E336" t="s">
-        <v>979</v>
+        <v>972</v>
       </c>
     </row>
     <row r="337" spans="1:3" hidden="1" x14ac:dyDescent="0.75">
@@ -9253,7 +9374,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="424" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="424" spans="1:5" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A424" s="6" t="s">
         <v>832</v>
       </c>
@@ -9267,7 +9388,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="425" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A425" s="4" t="s">
         <v>832</v>
       </c>
@@ -9281,7 +9402,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="426" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A426" s="4" t="s">
         <v>832</v>
       </c>
@@ -9295,7 +9416,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="427" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A427" s="4" t="s">
         <v>832</v>
       </c>
@@ -9309,10 +9430,10 @@
         <v>910</v>
       </c>
       <c r="E427" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.75">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A428" s="4" t="s">
         <v>832</v>
       </c>
@@ -9326,7 +9447,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="429" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A429" s="4" t="s">
         <v>832</v>
       </c>
@@ -9340,7 +9461,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="430" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="430" spans="1:5" ht="77.25" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A430" s="4" t="s">
         <v>832</v>
       </c>
@@ -9354,7 +9475,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="431" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A431" s="4" t="s">
         <v>832</v>
       </c>
@@ -9368,7 +9489,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="432" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A432" s="4" t="s">
         <v>832</v>
       </c>
@@ -9382,7 +9503,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="433" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A433" s="4" t="s">
         <v>832</v>
       </c>
@@ -9396,10 +9517,10 @@
         <v>911</v>
       </c>
       <c r="E433" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.75">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A434" s="4" t="s">
         <v>832</v>
       </c>
@@ -9413,10 +9534,10 @@
         <v>911</v>
       </c>
       <c r="E434" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.75">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="435" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A435" s="4" t="s">
         <v>832</v>
       </c>
@@ -9430,7 +9551,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="436" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="436" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A436" s="4" t="s">
         <v>832</v>
       </c>
@@ -9444,7 +9565,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="437" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A437" s="4" t="s">
         <v>832</v>
       </c>
@@ -9458,7 +9579,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="438" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="438" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A438" s="4" t="s">
         <v>832</v>
       </c>
@@ -9472,7 +9593,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="439" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="439" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A439" s="4" t="s">
         <v>832</v>
       </c>
@@ -9486,7 +9607,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="440" spans="1:5" ht="60.45" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="440" spans="1:5" ht="60.45" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A440" s="4" t="s">
         <v>832</v>
       </c>
@@ -9500,7 +9621,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="441" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A441" s="4" t="s">
         <v>832</v>
       </c>
@@ -9517,7 +9638,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="442" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="442" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A442" s="4" t="s">
         <v>832</v>
       </c>
@@ -9531,7 +9652,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="443" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A443" s="4" t="s">
         <v>832</v>
       </c>
@@ -9545,7 +9666,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="444" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A444" s="4" t="s">
         <v>832</v>
       </c>
@@ -9559,7 +9680,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="445" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A445" s="4" t="s">
         <v>832</v>
       </c>
@@ -9573,7 +9694,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="446" spans="1:5" s="9" customFormat="1" ht="59" x14ac:dyDescent="0.75">
+    <row r="446" spans="1:5" s="9" customFormat="1" ht="59" hidden="1" x14ac:dyDescent="0.75">
       <c r="A446" s="6" t="s">
         <v>832</v>
       </c>
@@ -9587,7 +9708,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="447" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A447" s="4" t="s">
         <v>832</v>
       </c>
@@ -9601,7 +9722,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="448" spans="1:5" ht="59" x14ac:dyDescent="0.75">
+    <row r="448" spans="1:5" ht="59" hidden="1" x14ac:dyDescent="0.75">
       <c r="A448" s="4" t="s">
         <v>832</v>
       </c>
@@ -9615,7 +9736,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="449" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="449" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A449" s="4" t="s">
         <v>832</v>
       </c>
@@ -9629,7 +9750,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="450" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="450" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A450" s="4" t="s">
         <v>832</v>
       </c>
@@ -9643,7 +9764,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="451" spans="1:5" ht="45.45" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="451" spans="1:5" ht="45.45" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A451" s="4" t="s">
         <v>832</v>
       </c>
@@ -9657,7 +9778,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="452" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="452" spans="1:5" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
       <c r="A452" s="6" t="s">
         <v>889</v>
       </c>
@@ -9671,7 +9792,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="453" spans="1:5" s="9" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="453" spans="1:5" s="9" customFormat="1" ht="30.45" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A453" s="6" t="s">
         <v>889</v>
       </c>
@@ -9685,7 +9806,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="454" spans="1:5" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="454" spans="1:5" s="9" customFormat="1" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A454" s="6" t="s">
         <v>889</v>
       </c>
@@ -9699,7 +9820,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="455" spans="1:5" s="9" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="455" spans="1:5" s="9" customFormat="1" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A455" s="6" t="s">
         <v>889</v>
       </c>
@@ -9713,7 +9834,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="456" spans="1:5" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="456" spans="1:5" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A456" s="6" t="s">
         <v>889</v>
       </c>
@@ -9727,7 +9848,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="457" spans="1:5" s="9" customFormat="1" ht="30.45" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="457" spans="1:5" s="9" customFormat="1" ht="30.45" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A457" s="6" t="s">
         <v>889</v>
       </c>
@@ -9741,7 +9862,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="458" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="458" spans="1:5" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A458" s="6" t="s">
         <v>889</v>
       </c>
@@ -9755,7 +9876,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="459" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="459" spans="1:5" ht="28.95" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A459" s="6" t="s">
         <v>889</v>
       </c>
@@ -9769,7 +9890,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="460" spans="1:5" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="460" spans="1:5" ht="32.700000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A460" s="6" t="s">
         <v>889</v>
       </c>
@@ -9783,7 +9904,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="461" spans="1:5" ht="23.7" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="461" spans="1:5" ht="23.7" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A461" s="6" t="s">
         <v>889</v>
       </c>
@@ -9797,7 +9918,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="462" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="462" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A462" s="6" t="s">
         <v>889</v>
       </c>
@@ -9811,7 +9932,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="463" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="463" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A463" s="6" t="s">
         <v>889</v>
       </c>
@@ -9825,10 +9946,10 @@
         <v>911</v>
       </c>
       <c r="E463" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="464" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A464" s="6" t="s">
         <v>832</v>
       </c>
@@ -9842,7 +9963,7 @@
         <v>911</v>
       </c>
       <c r="E464" t="s">
-        <v>977</v>
+        <v>970</v>
       </c>
     </row>
     <row r="465" spans="1:5" hidden="1" x14ac:dyDescent="0.75">
@@ -9856,7 +9977,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="466" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="466" spans="1:5" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
       <c r="A466" s="4" t="s">
         <v>7</v>
       </c>
@@ -9870,11 +9991,16 @@
         <v>911</v>
       </c>
       <c r="E466" t="s">
-        <v>997</v>
+        <v>989</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E466" xr:uid="{00252C19-57C4-4095-B3AB-85A45AD6EFCF}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="PolLimit1Building"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="3">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10093,19 +10219,22 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B2:F53"/>
+  <dimension ref="B2:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="2" max="2" width="21.86328125" customWidth="1"/>
-    <col min="3" max="3" width="15.6796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
     <col min="4" max="4" width="35.54296875" customWidth="1"/>
     <col min="5" max="5" width="59.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="26" x14ac:dyDescent="1.2">
@@ -10123,7 +10252,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B6" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.75">
@@ -10138,7 +10267,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B9" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.75">
@@ -10243,7 +10372,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.75">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.75">
       <c r="B17" t="s">
         <v>933</v>
       </c>
@@ -10260,7 +10389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.75">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.75">
       <c r="B18" t="s">
         <v>933</v>
       </c>
@@ -10277,7 +10406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.75">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.75">
       <c r="B19" t="s">
         <v>934</v>
       </c>
@@ -10294,232 +10423,380 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="18.5" x14ac:dyDescent="0.9">
+    <row r="21" spans="2:9" ht="18.5" x14ac:dyDescent="0.9">
       <c r="B21" s="21" t="s">
         <v>956</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B23" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B24" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B26" s="22" t="s">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B22" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B24" s="26" t="s">
+        <v>871</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>997</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>845</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>849</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>847</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>853</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>851</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B25" s="26" t="s">
+        <v>994</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>998</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B26" s="26" t="s">
+        <v>992</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>999</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B27" s="26" t="s">
+        <v>993</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B28" s="26" t="s">
+        <v>995</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B29" s="26" t="s">
+        <v>996</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H29" s="26" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.75">
+      <c r="B31" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B33" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B34" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B36" s="22" t="s">
         <v>958</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C36" s="22" t="s">
         <v>939</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D36" s="22" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B27">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B37">
         <v>1</v>
       </c>
-      <c r="C27">
+      <c r="C37">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D37" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B28">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B38">
         <v>2</v>
       </c>
-      <c r="C28">
+      <c r="C38">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D38" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B29">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B39">
         <v>3</v>
       </c>
-      <c r="C29">
+      <c r="C39">
         <v>1</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D39" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B30">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B40">
         <v>4</v>
       </c>
-      <c r="C30">
+      <c r="C40">
         <v>1</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D40" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B31">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B41">
         <v>5</v>
       </c>
-      <c r="C31">
+      <c r="C41">
         <v>2</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D41" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.75">
-      <c r="B32">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B42">
         <v>6</v>
       </c>
-      <c r="C32">
+      <c r="C42">
         <v>2</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D42" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B33">
-        <v>7</v>
-      </c>
-      <c r="C33">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="C43">
         <v>2</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D43" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B34">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B44">
         <v>8</v>
       </c>
-      <c r="C34">
+      <c r="C44">
         <v>2</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D44" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B35">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B45">
         <v>9</v>
       </c>
-      <c r="C35">
+      <c r="C45">
         <v>3</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D45" t="s">
         <v>947</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B37" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B38" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B39" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B40" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B41" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B42" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B44" s="1" t="s">
-        <v>929</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>935</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B45" t="s">
-        <v>963</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.75">
-      <c r="B46" t="s">
-        <v>962</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.75">
       <c r="B47" t="s">
-        <v>966</v>
-      </c>
-      <c r="C47">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B48" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B49" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B50" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B51" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B54" s="22" t="s">
+        <v>929</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>935</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B55" t="s">
+        <v>961</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B56" t="s">
+        <v>960</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B57" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C57">
         <v>3</v>
       </c>
-      <c r="D47" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="18.5" x14ac:dyDescent="0.9">
-      <c r="B50" s="21" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.75">
-      <c r="B51" t="s">
-        <v>991</v>
-      </c>
-      <c r="C51" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.75">
-      <c r="B52" t="s">
-        <v>986</v>
-      </c>
-      <c r="C52" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.75">
-      <c r="B53" t="s">
-        <v>990</v>
-      </c>
-      <c r="C53" t="s">
-        <v>989</v>
+      <c r="D57" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" ht="18.5" x14ac:dyDescent="0.9">
+      <c r="B60" s="21" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B61" t="s">
+        <v>983</v>
+      </c>
+      <c r="C61" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B62" t="s">
+        <v>978</v>
+      </c>
+      <c r="C62" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.75">
+      <c r="B63" t="s">
+        <v>982</v>
+      </c>
+      <c r="C63" t="s">
+        <v>981</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added support for OccAttachment for PR
</commit_message>
<xml_diff>
--- a/docs/OED_financial_terms_supported.xlsx
+++ b/docs/OED_financial_terms_supported.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\joh\Joh\07 Dev\FM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\joh\dev\OasisLMF_dev\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CE05FB-F7EF-4F9D-9A27-971763CB1572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2E1899-E60D-4685-81BA-F79BC3E2DA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="1043">
   <si>
     <t>File Name</t>
   </si>
@@ -3282,6 +3282,9 @@
   </si>
   <si>
     <t>Only supports Code=0 (default) and 2=Franchise</t>
+  </si>
+  <si>
+    <t>2.3.4</t>
   </si>
 </sst>
 </file>
@@ -3953,7 +3956,7 @@
   <dimension ref="B2:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3979,7 +3982,7 @@
       <c r="C6" s="19"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18" t="s">
-        <v>1032</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -11256,9 +11259,7 @@
   </sheetPr>
   <dimension ref="B2:J70"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11680,6 +11681,9 @@
       <c r="G35" t="s">
         <v>987</v>
       </c>
+      <c r="H35" t="s">
+        <v>987</v>
+      </c>
       <c r="I35" t="s">
         <v>987</v>
       </c>

</xml_diff>

<commit_message>
Added support for occurrence attachment for Per Risk XL (#1516)
* added support for occurrence attachment for Per Risk XoL

* added support for OccAttachment for PR
</commit_message>
<xml_diff>
--- a/docs/OED_financial_terms_supported.xlsx
+++ b/docs/OED_financial_terms_supported.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\joh\Joh\07 Dev\FM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\joh\dev\OasisLMF_dev\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CE05FB-F7EF-4F9D-9A27-971763CB1572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2E1899-E60D-4685-81BA-F79BC3E2DA47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E539D7C-9D32-4C67-A2B8-662594CF78CB}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="1043">
   <si>
     <t>File Name</t>
   </si>
@@ -3282,6 +3282,9 @@
   </si>
   <si>
     <t>Only supports Code=0 (default) and 2=Franchise</t>
+  </si>
+  <si>
+    <t>2.3.4</t>
   </si>
 </sst>
 </file>
@@ -3953,7 +3956,7 @@
   <dimension ref="B2:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3979,7 +3982,7 @@
       <c r="C6" s="19"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18" t="s">
-        <v>1032</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -11256,9 +11259,7 @@
   </sheetPr>
   <dimension ref="B2:J70"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11680,6 +11681,9 @@
       <c r="G35" t="s">
         <v>987</v>
       </c>
+      <c r="H35" t="s">
+        <v>987</v>
+      </c>
       <c r="I35" t="s">
         <v>987</v>
       </c>

</xml_diff>